<commit_message>
Condensed some stuff into helper functions
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.phillips\Documents\GitHub\Poker-Stats\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ABD058-D50C-483C-817E-DA7858C5210D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72B3C82-D32C-4769-98EC-26777B4C34BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bankrolls" sheetId="1" r:id="rId1"/>
@@ -6063,8 +6063,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Pre-Flop Stats</a:t>
+              <a:t>VPIP,</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Pre-flop raise, three-bet</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6403,37 +6408,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -9186,8 +9160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9511,7 +9485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -9789,8 +9763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added new stat: C-betting!
New stat alert! The long-sought C-bet percentage and count vs opportunities will now print with the other stats
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.phillips\Documents\GitHub\Poker-Stats\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0CBBA8-CDEA-40D2-8959-139D242E6863}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33E540A-3385-426F-A86D-7101A47EE816}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -130,7 +130,22 @@
     <t>Hands played</t>
   </si>
   <si>
-    <t>Xavier</t>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Kynan</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Marshall</t>
+  </si>
+  <si>
+    <t>Regan</t>
   </si>
 </sst>
 </file>
@@ -361,7 +376,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-83C5-4956-A2F6-D546348071B0}"/>
+              <c16:uniqueId val="{00000000-6558-4BBA-AB6E-C9C0695DDD78}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -460,7 +475,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-83C5-4956-A2F6-D546348071B0}"/>
+              <c16:uniqueId val="{00000001-6558-4BBA-AB6E-C9C0695DDD78}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -789,7 +804,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3C2C-4964-8B6B-7604AED95F1B}"/>
+              <c16:uniqueId val="{00000000-44F9-42AA-9971-EA334829DDAB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1038,7 +1053,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BD7C-48FC-A3C5-E273B7E4A928}"/>
+              <c16:uniqueId val="{00000000-3884-45CB-BCBA-A8ED4013D277}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1098,7 +1113,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BD7C-48FC-A3C5-E273B7E4A928}"/>
+              <c16:uniqueId val="{00000001-3884-45CB-BCBA-A8ED4013D277}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1158,7 +1173,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-BD7C-48FC-A3C5-E273B7E4A928}"/>
+              <c16:uniqueId val="{00000002-3884-45CB-BCBA-A8ED4013D277}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1482,7 +1497,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2784-44F2-8194-22846F4DE783}"/>
+              <c16:uniqueId val="{00000000-28E6-46AC-A03F-DCB79F847776}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1772,7 +1787,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1BBF-4ED5-AB9D-41314494DEFB}"/>
+              <c16:uniqueId val="{00000000-45D4-45DF-AA48-18D1307F76B5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1867,7 +1882,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1BBF-4ED5-AB9D-41314494DEFB}"/>
+              <c16:uniqueId val="{00000001-45D4-45DF-AA48-18D1307F76B5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2182,7 +2197,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FE71-4748-9C80-CD9977D5EDD8}"/>
+              <c16:uniqueId val="{00000000-45F3-4775-BB6C-D4F38322AE3D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2287,7 +2302,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FE71-4748-9C80-CD9977D5EDD8}"/>
+              <c16:uniqueId val="{00000001-45F3-4775-BB6C-D4F38322AE3D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2581,7 +2596,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A6DA-46E1-9A0A-CA46AEE373A7}"/>
+              <c16:uniqueId val="{00000000-D209-42F3-BF19-C66D279E6E0B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2777,9 +2792,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>VPIP</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2792,57 +2804,90 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'All Stats-this session'!$A$2:$A$5</c:f>
+              <c:f>'All Stats-this session'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Fish</c:v>
+                  <c:v>Scott</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Cedric</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scott</c:v>
+                  <c:v>Bill</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Xavier</c:v>
+                  <c:v>Kynan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jonathan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jacob</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Marshall</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Regan</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cheyenne</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'All Stats-this session'!$F$2:$F$5</c:f>
+              <c:f>'All Stats-this session'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.71099999999999997</c:v>
+                  <c:v>0.61699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.58599999999999997</c:v>
+                  <c:v>0.36199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.65700000000000003</c:v>
+                  <c:v>0.64800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.84699999999999998</c:v>
+                  <c:v>0.63600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.71699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.64600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.67500000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-104E-4A4F-B38E-0AD46BB260B9}"/>
+              <c16:uniqueId val="{00000000-6066-414F-AA77-4867F2E3DA22}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>PFR</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -2855,57 +2900,90 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'All Stats-this session'!$A$2:$A$5</c:f>
+              <c:f>'All Stats-this session'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Fish</c:v>
+                  <c:v>Scott</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Cedric</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scott</c:v>
+                  <c:v>Bill</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Xavier</c:v>
+                  <c:v>Kynan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jonathan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jacob</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Marshall</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Regan</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cheyenne</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'All Stats-this session'!$G$2:$G$5</c:f>
+              <c:f>'All Stats-this session'!$G$2:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.7999999999999999E-2</c:v>
+                  <c:v>0.40600000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.34300000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.49199999999999999</c:v>
+                <c:pt idx="7">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.28100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-104E-4A4F-B38E-0AD46BB260B9}"/>
+              <c16:uniqueId val="{00000001-6066-414F-AA77-4867F2E3DA22}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>3 Bet</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -2918,40 +2996,76 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'All Stats-this session'!$A$2:$A$5</c:f>
+              <c:f>'All Stats-this session'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Fish</c:v>
+                  <c:v>Scott</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Cedric</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scott</c:v>
+                  <c:v>Bill</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Xavier</c:v>
+                  <c:v>Kynan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jonathan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jacob</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Marshall</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Regan</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cheyenne</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'All Stats-this session'!$H$2:$H$5</c:f>
+              <c:f>'All Stats-this session'!$H$2:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3.9100000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5499999999999997E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.07E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2900000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2959,7 +3073,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-104E-4A4F-B38E-0AD46BB260B9}"/>
+              <c16:uniqueId val="{00000002-6066-414F-AA77-4867F2E3DA22}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3242,48 +3356,84 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'All Stats-this session'!$A$2:$A$5</c:f>
+              <c:f>'All Stats-this session'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Fish</c:v>
+                  <c:v>Scott</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Cedric</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scott</c:v>
+                  <c:v>Bill</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Xavier</c:v>
+                  <c:v>Kynan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jonathan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jacob</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Marshall</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Regan</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cheyenne</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'All Stats-this session'!$I$2:$I$5</c:f>
+              <c:f>'All Stats-this session'!$I$2:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.44</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.89</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.67</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.42</c:v>
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7172-48E3-B01B-038B17B7049A}"/>
+              <c16:uniqueId val="{00000000-87E7-4D0C-A031-FF0EA4F59B1F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3532,48 +3682,84 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'All Stats-this session'!$A$2:$A$5</c:f>
+              <c:f>'All Stats-this session'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Fish</c:v>
+                  <c:v>Scott</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Cedric</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scott</c:v>
+                  <c:v>Bill</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Xavier</c:v>
+                  <c:v>Kynan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jonathan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jacob</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Marshall</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Regan</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cheyenne</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'All Stats-this session'!$K$2:$K$5</c:f>
+              <c:f>'All Stats-this session'!$K$2:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.30299999999999999</c:v>
+                  <c:v>0.22700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27600000000000002</c:v>
+                  <c:v>0.106</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16</c:v>
+                  <c:v>0.214</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45800000000000002</c:v>
+                  <c:v>0.17799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-833C-42BE-A28E-C75D490346F6}"/>
+              <c16:uniqueId val="{00000000-7840-40EF-91AC-4AAF0255240B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3627,48 +3813,84 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'All Stats-this session'!$A$2:$A$5</c:f>
+              <c:f>'All Stats-this session'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Fish</c:v>
+                  <c:v>Scott</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Cedric</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scott</c:v>
+                  <c:v>Bill</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Xavier</c:v>
+                  <c:v>Kynan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jonathan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jacob</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Marshall</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Regan</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cheyenne</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'All Stats-this session'!$L$2:$L$5</c:f>
+              <c:f>'All Stats-this session'!$L$2:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.16500000000000001</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.124</c:v>
+                  <c:v>5.7000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.107</c:v>
+                  <c:v>9.7000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13600000000000001</c:v>
+                  <c:v>7.8E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-833C-42BE-A28E-C75D490346F6}"/>
+              <c16:uniqueId val="{00000001-7840-40EF-91AC-4AAF0255240B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3942,48 +4164,84 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'All Stats-this session'!$A$2:$A$5</c:f>
+              <c:f>'All Stats-this session'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Fish</c:v>
+                  <c:v>Scott</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Cedric</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scott</c:v>
+                  <c:v>Bill</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Xavier</c:v>
+                  <c:v>Kynan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jonathan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jacob</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Marshall</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Regan</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cheyenne</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'All Stats-this session'!$M$2:$M$5</c:f>
+              <c:f>'All Stats-this session'!$M$2:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>161.46</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>159.28</c:v>
+                  <c:v>48.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>190.59</c:v>
+                  <c:v>322.52999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.38</c:v>
+                  <c:v>48.56</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>393.14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>147.59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>121.03</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-564E-4762-B1D8-E383B0DAFF02}"/>
+              <c16:uniqueId val="{00000000-FAFF-4B79-94E0-3DCE5F8B1BED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4047,48 +4305,84 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'All Stats-this session'!$A$2:$A$5</c:f>
+              <c:f>'All Stats-this session'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Fish</c:v>
+                  <c:v>Scott</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Cedric</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scott</c:v>
+                  <c:v>Bill</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Xavier</c:v>
+                  <c:v>Kynan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jonathan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jacob</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Marshall</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Regan</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cheyenne</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'All Stats-this session'!$N$2:$N$5</c:f>
+              <c:f>'All Stats-this session'!$N$2:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>79.63</c:v>
+                  <c:v>37.68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.6</c:v>
+                  <c:v>8.15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96.96</c:v>
+                  <c:v>13.92</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.1</c:v>
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.07</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>49.87</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-564E-4762-B1D8-E383B0DAFF02}"/>
+              <c16:uniqueId val="{00000001-FAFF-4B79-94E0-3DCE5F8B1BED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4381,7 +4675,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-53BE-4498-80C9-329EEC6DB226}"/>
+              <c16:uniqueId val="{00000000-B083-40C0-88EF-DCAEDA258E2A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4480,7 +4774,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-53BE-4498-80C9-329EEC6DB226}"/>
+              <c16:uniqueId val="{00000001-B083-40C0-88EF-DCAEDA258E2A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4731,48 +5025,84 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'All Stats-this session'!$A$2:$A$5</c:f>
+              <c:f>'All Stats-this session'!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Fish</c:v>
+                  <c:v>Scott</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Cedric</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scott</c:v>
+                  <c:v>Bill</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Xavier</c:v>
+                  <c:v>Kynan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jonathan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jacob</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Marshall</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Regan</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Cheyenne</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'All Stats-this session'!$O$2:$O$5</c:f>
+              <c:f>'All Stats-this session'!$O$2:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>218</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>210</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>169</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59</c:v>
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8BDD-427B-A4D4-6170378ED4CD}"/>
+              <c16:uniqueId val="{00000000-79A1-4383-B935-953DD5786AC4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5064,7 +5394,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2EDC-45ED-B942-5FD39EACC258}"/>
+              <c16:uniqueId val="{00000000-E266-4F8B-B265-E5CE1260F7ED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5163,7 +5493,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2EDC-45ED-B942-5FD39EACC258}"/>
+              <c16:uniqueId val="{00000001-E266-4F8B-B265-E5CE1260F7ED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5454,7 +5784,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8A7F-46C4-915A-83FAD9C8780A}"/>
+              <c16:uniqueId val="{00000000-D98C-40C3-8E5C-2A6FD570090D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5553,7 +5883,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8A7F-46C4-915A-83FAD9C8780A}"/>
+              <c16:uniqueId val="{00000001-D98C-40C3-8E5C-2A6FD570090D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5844,7 +6174,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C8CF-4D26-9556-7809AE098A1E}"/>
+              <c16:uniqueId val="{00000000-6894-494D-A4F8-395C428546D2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5943,7 +6273,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C8CF-4D26-9556-7809AE098A1E}"/>
+              <c16:uniqueId val="{00000001-6894-494D-A4F8-395C428546D2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6202,7 +6532,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0467-4D5F-88B8-8B67A171A47D}"/>
+              <c16:uniqueId val="{00000000-BE00-4BE3-952C-9565AB50B297}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6268,7 +6598,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0467-4D5F-88B8-8B67A171A47D}"/>
+              <c16:uniqueId val="{00000001-BE00-4BE3-952C-9565AB50B297}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6334,7 +6664,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0467-4D5F-88B8-8B67A171A47D}"/>
+              <c16:uniqueId val="{00000002-BE00-4BE3-952C-9565AB50B297}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6633,7 +6963,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-06AF-4F41-B8EE-A4778E252BEA}"/>
+              <c16:uniqueId val="{00000000-2FD7-495D-BE1C-FDFA572AA70F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6929,7 +7259,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CDD4-47CA-9600-3026AB92AE90}"/>
+              <c16:uniqueId val="{00000000-6A68-41D8-AD12-9CBEC3FD2539}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7030,7 +7360,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CDD4-47CA-9600-3026AB92AE90}"/>
+              <c16:uniqueId val="{00000001-6A68-41D8-AD12-9CBEC3FD2539}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7351,7 +7681,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-33FC-4A93-A87E-9E45CFD137CD}"/>
+              <c16:uniqueId val="{00000000-B7E5-48EA-B90A-90527ECE4360}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7462,7 +7792,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-33FC-4A93-A87E-9E45CFD137CD}"/>
+              <c16:uniqueId val="{00000001-B7E5-48EA-B90A-90527ECE4360}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9267,7 +9597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
@@ -9868,10 +10198,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9944,49 +10274,49 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>46.46</v>
+      </c>
+      <c r="D2" s="2">
+        <v>6.46</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>26.14</v>
-      </c>
-      <c r="D2" s="2">
-        <v>6.14</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
       <c r="F2">
-        <v>0.71099999999999997</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="G2">
-        <v>1.7999999999999999E-2</v>
+        <v>0.40600000000000003</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>3.9100000000000003E-2</v>
       </c>
       <c r="I2">
-        <v>0.44</v>
+        <v>1.7</v>
       </c>
       <c r="J2">
-        <v>0.22800000000000001</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="K2">
-        <v>0.30299999999999999</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="L2">
-        <v>0.16500000000000001</v>
+        <v>0.125</v>
       </c>
       <c r="M2">
-        <v>161.46</v>
+        <v>147</v>
       </c>
       <c r="N2">
-        <v>79.63</v>
+        <v>37.68</v>
       </c>
       <c r="O2">
-        <v>218</v>
+        <v>128</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="3"/>
@@ -9996,145 +10326,427 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C3">
-        <v>12.39</v>
+        <v>22.25</v>
       </c>
       <c r="D3" s="2">
-        <v>-7.61</v>
+        <v>-7.75</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.58599999999999997</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0.89</v>
+        <v>0.39</v>
       </c>
       <c r="J3">
-        <v>0.3</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="K3">
-        <v>0.27600000000000002</v>
+        <v>0.106</v>
       </c>
       <c r="L3">
-        <v>0.124</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="M3">
-        <v>159.28</v>
+        <v>48.54</v>
       </c>
       <c r="N3">
-        <v>54.6</v>
+        <v>8.15</v>
       </c>
       <c r="O3">
-        <v>210</v>
+        <v>141</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="3"/>
       <c r="T3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>55.27</v>
+        <v>66.010000000000005</v>
       </c>
       <c r="D4" s="2">
-        <v>35.270000000000003</v>
+        <v>36.01</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="G4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0.65700000000000003</v>
-      </c>
-      <c r="G4">
-        <v>0.34300000000000003</v>
-      </c>
-      <c r="H4">
-        <v>3.5499999999999997E-2</v>
-      </c>
       <c r="I4">
-        <v>3.67</v>
+        <v>0.52</v>
       </c>
       <c r="J4">
-        <v>0.54300000000000004</v>
+        <v>0.219</v>
       </c>
       <c r="K4">
-        <v>0.16</v>
+        <v>0.214</v>
       </c>
       <c r="L4">
-        <v>0.107</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="M4">
-        <v>190.59</v>
+        <v>322.52999999999997</v>
       </c>
       <c r="N4">
-        <v>96.96</v>
+        <v>13.92</v>
       </c>
       <c r="O4">
-        <v>169</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>-50</v>
+        <v>-30</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5">
-        <v>0.84699999999999998</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="G5">
-        <v>0.49199999999999999</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1.42</v>
+        <v>0.26</v>
       </c>
       <c r="J5">
-        <v>0.47699999999999998</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="K5">
-        <v>0.45800000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="L5">
-        <v>0.13600000000000001</v>
+        <v>7.8E-2</v>
       </c>
       <c r="M5">
-        <v>74.38</v>
+        <v>48.56</v>
       </c>
       <c r="N5">
-        <v>27.1</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="O5">
-        <v>59</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>19.510000000000002</v>
+      </c>
+      <c r="D6">
+        <v>-0.49</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="G6">
+        <v>2.3E-2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0.24</v>
+      </c>
+      <c r="J6">
+        <v>0.11</v>
+      </c>
+      <c r="K6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M6">
+        <v>10.52</v>
+      </c>
+      <c r="N6">
+        <v>6.95</v>
+      </c>
+      <c r="O6">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>185.77</v>
+      </c>
+      <c r="D7">
+        <v>155.77000000000001</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="G7">
+        <v>5.5E-2</v>
+      </c>
+      <c r="H7">
+        <v>2.07E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.18</v>
+      </c>
+      <c r="J7">
+        <v>0.107</v>
+      </c>
+      <c r="K7">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="L7">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="M7">
+        <v>393.14</v>
+      </c>
+      <c r="N7">
+        <v>13.71</v>
+      </c>
+      <c r="O7">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>-20</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0.22</v>
+      </c>
+      <c r="J8">
+        <v>0.108</v>
+      </c>
+      <c r="K8">
+        <v>0.152</v>
+      </c>
+      <c r="L8">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="M8">
+        <v>48.5</v>
+      </c>
+      <c r="N8">
+        <v>18.2</v>
+      </c>
+      <c r="O8">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>-10</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="G9">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0.23</v>
+      </c>
+      <c r="J9">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="K9">
+        <v>0.26</v>
+      </c>
+      <c r="L9">
+        <v>0.125</v>
+      </c>
+      <c r="M9">
+        <v>147.59</v>
+      </c>
+      <c r="N9">
+        <v>38.07</v>
+      </c>
+      <c r="O9">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>120</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>-120</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="G10">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="H10">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="I10">
+        <v>1.38</v>
+      </c>
+      <c r="J10">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="K10">
+        <v>0.25</v>
+      </c>
+      <c r="L10">
+        <v>9.4E-2</v>
+      </c>
+      <c r="M10">
+        <v>121.03</v>
+      </c>
+      <c r="N10">
+        <v>49.87</v>
+      </c>
+      <c r="O10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>-10</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="G11">
+        <v>0.05</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0.25</v>
+      </c>
+      <c r="J11">
+        <v>0.12</v>
+      </c>
+      <c r="K11">
+        <v>0.2</v>
+      </c>
+      <c r="L11">
+        <v>0.1</v>
+      </c>
+      <c r="M11">
+        <v>10.94</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparing to put outputs in diff script
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -406,7 +406,6 @@
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -516,7 +515,6 @@
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -623,7 +621,6 @@
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -733,7 +730,6 @@
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -8089,6 +8085,430 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>VPIP, Pre-flop raise, 3-bet</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!F1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$F$2:$F$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!G1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$G$2:$G$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!H1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$H$2:$H$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Aggression Factor</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!L1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$L$2:$L$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>C-bets vs opportunities</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!M1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$M$2:$M$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!N1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$N$2:$N$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="b"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Went to showdown vs Won at showdown</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!J1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$J$2:$J$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!K1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$K$2:$K$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
@@ -8329,6 +8749,818 @@
         <crossAx val="10"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Money won</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!O1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$O$2:$O$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!P1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$P$2:$P$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="b"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Hands played</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="bar"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!Q1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$Q$2:$Q$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart52.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>VPIP, Pre-flop raise, 3-bet</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!F1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$F$2:$F$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!G1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$G$2:$G$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!H1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$H$2:$H$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Aggression Factor</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!L1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$L$2:$L$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>C-bets vs opportunities</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!M1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$M$2:$M$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!N1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$N$2:$N$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="b"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Went to showdown vs Won at showdown</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!J1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$J$2:$J$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!K1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$K$2:$K$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart56.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Money won</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!O1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$O$2:$O$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!P1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$P$2:$P$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="b"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Hands played</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="bar"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'All Stats-this session'!Q1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'All Stats-this session'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'All Stats-this session'!$Q$2:$Q$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
       </valAx>
     </plotArea>
     <plotVisOnly val="1"/>
@@ -8755,7 +9987,6 @@
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -8883,7 +10114,6 @@
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -9966,6 +11196,270 @@
     </graphicFrame>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>13</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8640000" cy="4860000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="33" name="Chart 33"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId33"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>13</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8640000" cy="4860000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="34" name="Chart 34"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId34"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8640000" cy="4860000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="35" name="Chart 35"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId35"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8640000" cy="4860000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="36" name="Chart 36"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId36"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>65</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8640000" cy="4860000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="37" name="Chart 37"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId37"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>65</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="4680000" cy="4680000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="38" name="Chart 38"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId38"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>13</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8640000" cy="4860000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="39" name="Chart 39"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId39"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>13</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8640000" cy="4860000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="40" name="Chart 40"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId40"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8640000" cy="4860000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="41" name="Chart 41"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId41"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8640000" cy="4860000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="42" name="Chart 42"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId42"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>65</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8640000" cy="4860000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="43" name="Chart 43"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId43"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>65</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="4680000" cy="4680000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="44" name="Chart 44"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId44"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -11267,7 +12761,7 @@
       <c r="S3" s="2" t="n"/>
       <c r="T3" t="inlineStr">
         <is>
-          <t>6 07</t>
+          <t>0607</t>
         </is>
       </c>
       <c r="AF3" t="n">

</xml_diff>

<commit_message>
Resolved graph overlap issue
Charts were previously stacking on top of each other on every run where stats from current session are filled.

This commit solves this Github issue by deleting the old sheet and creating a new one to fill completely from scratch with the requested data.
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -6,9 +6,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NL Stats-this session" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="combined Stats-this session" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="PLO Stats-this session" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="All Stats-this session" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="NL Stats-this session" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -17,10 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00_-"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_-"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -51,27 +50,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -150,6 +132,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -175,7 +158,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!F1</f>
+              <f>'combined Stats-this session'!F1</f>
             </strRef>
           </tx>
           <spPr>
@@ -185,12 +168,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$F$2:$F$6</f>
+              <f>'combined Stats-this session'!$F$2:$F$11</f>
             </numRef>
           </val>
         </ser>
@@ -199,7 +182,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!G1</f>
+              <f>'combined Stats-this session'!G1</f>
             </strRef>
           </tx>
           <spPr>
@@ -209,12 +192,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$G$2:$G$6</f>
+              <f>'combined Stats-this session'!$G$2:$G$11</f>
             </numRef>
           </val>
         </ser>
@@ -223,7 +206,7 @@
           <order val="2"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!H1</f>
+              <f>'combined Stats-this session'!H1</f>
             </strRef>
           </tx>
           <spPr>
@@ -233,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$H$2:$H$6</f>
+              <f>'combined Stats-this session'!$H$2:$H$11</f>
             </numRef>
           </val>
         </ser>
@@ -277,7 +260,6 @@
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -384,7 +366,6 @@
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -494,7 +475,6 @@
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -582,27 +562,38 @@
       <tx>
         <rich>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>VPIP, Pre-flop raise, 3-bet</a:t>
             </a:r>
           </a:p>
         </rich>
       </tx>
+      <overlay val="0"/>
     </title>
     <plotArea>
+      <layout/>
       <barChart>
         <barDir val="col"/>
         <grouping val="clustered"/>
+        <varyColors val="0"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'All Stats-this session'!F1</f>
+              <f>'NL Stats-this session'!$F$1</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>VPIP</v>
+                </pt>
+              </strCache>
             </strRef>
           </tx>
           <spPr>
@@ -610,14 +601,52 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
+          <invertIfNegative val="0"/>
           <cat>
-            <numRef>
-              <f>'All Stats-this session'!$A$2:$A$6</f>
-            </numRef>
+            <strRef>
+              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Fish</v>
+                </pt>
+                <pt idx="1">
+                  <v>Scott</v>
+                </pt>
+                <pt idx="2">
+                  <v>Raymond</v>
+                </pt>
+                <pt idx="3">
+                  <v>Jonathan</v>
+                </pt>
+                <pt idx="4">
+                  <v>Cedric</v>
+                </pt>
+              </strCache>
+            </strRef>
           </cat>
           <val>
             <numRef>
-              <f>'All Stats-this session'!$F$2:$F$6</f>
+              <f>'NL Stats-this session'!$F$2:$F$6</f>
+              <numCache>
+                <formatCode>0.0%</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>0.632</v>
+                </pt>
+                <pt idx="1">
+                  <v>0.7</v>
+                </pt>
+                <pt idx="2">
+                  <v>0.324</v>
+                </pt>
+                <pt idx="3">
+                  <v>0.371</v>
+                </pt>
+                <pt idx="4">
+                  <v>0.375</v>
+                </pt>
+              </numCache>
             </numRef>
           </val>
         </ser>
@@ -626,7 +655,13 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'All Stats-this session'!G1</f>
+              <f>'NL Stats-this session'!$G$1</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>Pre-flop Raise</v>
+                </pt>
+              </strCache>
             </strRef>
           </tx>
           <spPr>
@@ -634,14 +669,52 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
+          <invertIfNegative val="0"/>
           <cat>
-            <numRef>
-              <f>'All Stats-this session'!$A$2:$A$6</f>
-            </numRef>
+            <strRef>
+              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Fish</v>
+                </pt>
+                <pt idx="1">
+                  <v>Scott</v>
+                </pt>
+                <pt idx="2">
+                  <v>Raymond</v>
+                </pt>
+                <pt idx="3">
+                  <v>Jonathan</v>
+                </pt>
+                <pt idx="4">
+                  <v>Cedric</v>
+                </pt>
+              </strCache>
+            </strRef>
           </cat>
           <val>
             <numRef>
-              <f>'All Stats-this session'!$G$2:$G$6</f>
+              <f>'NL Stats-this session'!$G$2:$G$6</f>
+              <numCache>
+                <formatCode>0.0%</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>0.018</v>
+                </pt>
+                <pt idx="1">
+                  <v>0.459</v>
+                </pt>
+                <pt idx="2">
+                  <v>0.147</v>
+                </pt>
+                <pt idx="3">
+                  <v>0</v>
+                </pt>
+                <pt idx="4">
+                  <v>0.013</v>
+                </pt>
+              </numCache>
             </numRef>
           </val>
         </ser>
@@ -650,7 +723,13 @@
           <order val="2"/>
           <tx>
             <strRef>
-              <f>'All Stats-this session'!H1</f>
+              <f>'NL Stats-this session'!$H$1</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>Three-bet</v>
+                </pt>
+              </strCache>
             </strRef>
           </tx>
           <spPr>
@@ -658,17 +737,63 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
+          <invertIfNegative val="0"/>
           <cat>
-            <numRef>
-              <f>'All Stats-this session'!$A$2:$A$6</f>
-            </numRef>
+            <strRef>
+              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Fish</v>
+                </pt>
+                <pt idx="1">
+                  <v>Scott</v>
+                </pt>
+                <pt idx="2">
+                  <v>Raymond</v>
+                </pt>
+                <pt idx="3">
+                  <v>Jonathan</v>
+                </pt>
+                <pt idx="4">
+                  <v>Cedric</v>
+                </pt>
+              </strCache>
+            </strRef>
           </cat>
           <val>
             <numRef>
-              <f>'All Stats-this session'!$H$2:$H$6</f>
+              <f>'NL Stats-this session'!$H$2:$H$6</f>
+              <numCache>
+                <formatCode>0.0%</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>0</v>
+                </pt>
+                <pt idx="1">
+                  <v>0.06469999999999999</v>
+                </pt>
+                <pt idx="2">
+                  <v>0.0353</v>
+                </pt>
+                <pt idx="3">
+                  <v>0</v>
+                </pt>
+                <pt idx="4">
+                  <v>0</v>
+                </pt>
+              </numCache>
             </numRef>
           </val>
         </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
         <gapWidth val="150"/>
         <axId val="10"/>
         <axId val="100"/>
@@ -678,22 +803,34 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <axPos val="l"/>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
         <crossAx val="100"/>
+        <crosses val="autoZero"/>
+        <auto val="0"/>
+        <lblAlgn val="ctr"/>
         <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
+        <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
+        <numFmt formatCode="0.0%" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
         <crossAx val="10"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
       </valAx>
     </plotArea>
     <plotVisOnly val="1"/>
@@ -704,6 +841,1087 @@
 
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Aggression Factor</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <overlay val="0"/>
+    </title>
+    <plotArea>
+      <layout/>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'NL Stats-this session'!$L$1</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>Won at showdown</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <dLbls>
+            <spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+            <showLegendKey val="0"/>
+            <showVal val="1"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showBubbleSize val="0"/>
+            <showLeaderLines val="0"/>
+          </dLbls>
+          <cat>
+            <strRef>
+              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Fish</v>
+                </pt>
+                <pt idx="1">
+                  <v>Scott</v>
+                </pt>
+                <pt idx="2">
+                  <v>Raymond</v>
+                </pt>
+                <pt idx="3">
+                  <v>Jonathan</v>
+                </pt>
+                <pt idx="4">
+                  <v>Cedric</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'NL Stats-this session'!$L$2:$L$6</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>0.27</v>
+                </pt>
+                <pt idx="1">
+                  <v>4.15</v>
+                </pt>
+                <pt idx="2">
+                  <v>1.15</v>
+                </pt>
+                <pt idx="3">
+                  <v>0.12</v>
+                </pt>
+                <pt idx="4">
+                  <v>0.46</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="100"/>
+        <crosses val="autoZero"/>
+        <auto val="0"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="10"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>C-bets vs opportunities</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <overlay val="0"/>
+    </title>
+    <plotArea>
+      <layout/>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'NL Stats-this session'!$M$1</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>C-bets</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <dLbls>
+            <spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+            <showLegendKey val="0"/>
+            <showVal val="1"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showBubbleSize val="0"/>
+            <showLeaderLines val="0"/>
+          </dLbls>
+          <cat>
+            <strRef>
+              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Fish</v>
+                </pt>
+                <pt idx="1">
+                  <v>Scott</v>
+                </pt>
+                <pt idx="2">
+                  <v>Raymond</v>
+                </pt>
+                <pt idx="3">
+                  <v>Jonathan</v>
+                </pt>
+                <pt idx="4">
+                  <v>Cedric</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'NL Stats-this session'!$M$2:$M$6</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>1</v>
+                </pt>
+                <pt idx="1">
+                  <v>45</v>
+                </pt>
+                <pt idx="2">
+                  <v>9</v>
+                </pt>
+                <pt idx="3">
+                  <v>0</v>
+                </pt>
+                <pt idx="4">
+                  <v>2</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'NL Stats-this session'!$N$1</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>C-bet opportunities</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <dLbls>
+            <spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+            <showLegendKey val="0"/>
+            <showVal val="1"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showBubbleSize val="0"/>
+            <showLeaderLines val="0"/>
+          </dLbls>
+          <cat>
+            <strRef>
+              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Fish</v>
+                </pt>
+                <pt idx="1">
+                  <v>Scott</v>
+                </pt>
+                <pt idx="2">
+                  <v>Raymond</v>
+                </pt>
+                <pt idx="3">
+                  <v>Jonathan</v>
+                </pt>
+                <pt idx="4">
+                  <v>Cedric</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'NL Stats-this session'!$N$2:$N$6</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>5</v>
+                </pt>
+                <pt idx="1">
+                  <v>70</v>
+                </pt>
+                <pt idx="2">
+                  <v>24</v>
+                </pt>
+                <pt idx="3">
+                  <v>0</v>
+                </pt>
+                <pt idx="4">
+                  <v>2</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="100"/>
+        <crosses val="autoZero"/>
+        <auto val="0"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="10"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="b"/>
+      <overlay val="0"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Went to showdown vs Won at showdown</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <overlay val="0"/>
+    </title>
+    <plotArea>
+      <layout/>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'NL Stats-this session'!$J$1</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>Aggro Frequency</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <dLbls>
+            <spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+            <showLegendKey val="0"/>
+            <showVal val="1"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showBubbleSize val="0"/>
+            <showLeaderLines val="0"/>
+          </dLbls>
+          <cat>
+            <strRef>
+              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Fish</v>
+                </pt>
+                <pt idx="1">
+                  <v>Scott</v>
+                </pt>
+                <pt idx="2">
+                  <v>Raymond</v>
+                </pt>
+                <pt idx="3">
+                  <v>Jonathan</v>
+                </pt>
+                <pt idx="4">
+                  <v>Cedric</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'NL Stats-this session'!$J$2:$J$6</f>
+              <numCache>
+                <formatCode>0.0%</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>0.135</v>
+                </pt>
+                <pt idx="1">
+                  <v>0.124</v>
+                </pt>
+                <pt idx="2">
+                  <v>0.106</v>
+                </pt>
+                <pt idx="3">
+                  <v>0.081</v>
+                </pt>
+                <pt idx="4">
+                  <v>0.062</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'NL Stats-this session'!$K$1</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>Went to showdown</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <dLbls>
+            <spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+            <showLegendKey val="0"/>
+            <showVal val="1"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showBubbleSize val="0"/>
+            <showLeaderLines val="0"/>
+          </dLbls>
+          <cat>
+            <strRef>
+              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Fish</v>
+                </pt>
+                <pt idx="1">
+                  <v>Scott</v>
+                </pt>
+                <pt idx="2">
+                  <v>Raymond</v>
+                </pt>
+                <pt idx="3">
+                  <v>Jonathan</v>
+                </pt>
+                <pt idx="4">
+                  <v>Cedric</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'NL Stats-this session'!$K$2:$K$6</f>
+              <numCache>
+                <formatCode>0.0%</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>0.067</v>
+                </pt>
+                <pt idx="1">
+                  <v>0.047</v>
+                </pt>
+                <pt idx="2">
+                  <v>0.065</v>
+                </pt>
+                <pt idx="3">
+                  <v>0.04</v>
+                </pt>
+                <pt idx="4">
+                  <v>0.037</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="100"/>
+        <crosses val="autoZero"/>
+        <auto val="0"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <numFmt formatCode="0.0%" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="10"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Money won</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <overlay val="0"/>
+    </title>
+    <plotArea>
+      <layout/>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'NL Stats-this session'!$O$1</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>At showdown</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <dLbls>
+            <spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+            <showLegendKey val="0"/>
+            <showVal val="1"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showBubbleSize val="0"/>
+            <showLeaderLines val="0"/>
+          </dLbls>
+          <cat>
+            <strRef>
+              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Fish</v>
+                </pt>
+                <pt idx="1">
+                  <v>Scott</v>
+                </pt>
+                <pt idx="2">
+                  <v>Raymond</v>
+                </pt>
+                <pt idx="3">
+                  <v>Jonathan</v>
+                </pt>
+                <pt idx="4">
+                  <v>Cedric</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'NL Stats-this session'!$O$2:$O$6</f>
+              <numCache>
+                <formatCode>"$"#,##0.00_-</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>63.76</v>
+                </pt>
+                <pt idx="1">
+                  <v>109.4</v>
+                </pt>
+                <pt idx="2">
+                  <v>61.34</v>
+                </pt>
+                <pt idx="3">
+                  <v>6.68</v>
+                </pt>
+                <pt idx="4">
+                  <v>55.78</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'NL Stats-this session'!$P$1</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>Before showdown</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <dLbls>
+            <spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+            <showLegendKey val="0"/>
+            <showVal val="1"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showBubbleSize val="0"/>
+            <showLeaderLines val="0"/>
+          </dLbls>
+          <cat>
+            <strRef>
+              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Fish</v>
+                </pt>
+                <pt idx="1">
+                  <v>Scott</v>
+                </pt>
+                <pt idx="2">
+                  <v>Raymond</v>
+                </pt>
+                <pt idx="3">
+                  <v>Jonathan</v>
+                </pt>
+                <pt idx="4">
+                  <v>Cedric</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'NL Stats-this session'!$P$2:$P$6</f>
+              <numCache>
+                <formatCode>"$"#,##0.00_-</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>40.99</v>
+                </pt>
+                <pt idx="1">
+                  <v>157.65</v>
+                </pt>
+                <pt idx="2">
+                  <v>66.23999999999999</v>
+                </pt>
+                <pt idx="3">
+                  <v>11.4</v>
+                </pt>
+                <pt idx="4">
+                  <v>82.09</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="100"/>
+        <crosses val="autoZero"/>
+        <auto val="0"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <numFmt formatCode="&quot;$&quot;#,##0.00_-" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="10"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="b"/>
+      <overlay val="0"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Hands played</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <overlay val="0"/>
+    </title>
+    <plotArea>
+      <layout/>
+      <barChart>
+        <barDir val="bar"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'NL Stats-this session'!$Q$1</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>Hands played</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <dLbls>
+            <spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+            <showLegendKey val="0"/>
+            <showVal val="1"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showBubbleSize val="0"/>
+            <showLeaderLines val="0"/>
+          </dLbls>
+          <cat>
+            <strRef>
+              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Fish</v>
+                </pt>
+                <pt idx="1">
+                  <v>Scott</v>
+                </pt>
+                <pt idx="2">
+                  <v>Raymond</v>
+                </pt>
+                <pt idx="3">
+                  <v>Jonathan</v>
+                </pt>
+                <pt idx="4">
+                  <v>Cedric</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'NL Stats-this session'!$Q$2:$Q$6</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>163</v>
+                </pt>
+                <pt idx="1">
+                  <v>170</v>
+                </pt>
+                <pt idx="2">
+                  <v>170</v>
+                </pt>
+                <pt idx="3">
+                  <v>124</v>
+                </pt>
+                <pt idx="4">
+                  <v>160</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="1"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="100"/>
+        <crosses val="autoZero"/>
+        <auto val="0"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <majorGridlines/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="10"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -729,7 +1947,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'All Stats-this session'!L1</f>
+              <f>'combined Stats-this session'!L1</f>
             </strRef>
           </tx>
           <spPr>
@@ -739,500 +1957,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'All Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'All Stats-this session'!$L$2:$L$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <dLbls>
-          <showVal val="1"/>
-        </dLbls>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>C-bets vs opportunities</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'All Stats-this session'!M1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'All Stats-this session'!$A$2:$A$6</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'All Stats-this session'!$M$2:$M$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'All Stats-this session'!N1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'All Stats-this session'!$A$2:$A$6</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'All Stats-this session'!$N$2:$N$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <dLbls>
-          <showVal val="1"/>
-        </dLbls>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="b"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Went to showdown vs Won at showdown</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'All Stats-this session'!J1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'All Stats-this session'!$A$2:$A$6</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'All Stats-this session'!$J$2:$J$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'All Stats-this session'!K1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'All Stats-this session'!$A$2:$A$6</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'All Stats-this session'!$K$2:$K$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <dLbls>
-          <showVal val="1"/>
-        </dLbls>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Money won</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'All Stats-this session'!O1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'All Stats-this session'!$A$2:$A$6</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'All Stats-this session'!$O$2:$O$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'All Stats-this session'!P1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'All Stats-this session'!$A$2:$A$6</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'All Stats-this session'!$P$2:$P$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <dLbls>
-          <showVal val="1"/>
-        </dLbls>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="b"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Hands played</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="bar"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'All Stats-this session'!Q1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'All Stats-this session'!$A$2:$A$6</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'All Stats-this session'!$Q$2:$Q$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <dLbls>
-          <showVal val="1"/>
-        </dLbls>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Aggression Factor</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'NL Stats-this session'!L1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'NL Stats-this session'!$L$2:$L$6</f>
+              <f>'combined Stats-this session'!$L$2:$L$11</f>
             </numRef>
           </val>
         </ser>
@@ -1274,6 +2004,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -1299,7 +2030,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!M1</f>
+              <f>'combined Stats-this session'!M1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1309,12 +2040,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$M$2:$M$6</f>
+              <f>'combined Stats-this session'!$M$2:$M$11</f>
             </numRef>
           </val>
         </ser>
@@ -1323,7 +2054,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!N1</f>
+              <f>'combined Stats-this session'!N1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1333,12 +2064,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$N$2:$N$6</f>
+              <f>'combined Stats-this session'!$N$2:$N$11</f>
             </numRef>
           </val>
         </ser>
@@ -1383,6 +2114,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -1408,7 +2140,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!J1</f>
+              <f>'combined Stats-this session'!J1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1418,12 +2150,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$J$2:$J$6</f>
+              <f>'combined Stats-this session'!$J$2:$J$11</f>
             </numRef>
           </val>
         </ser>
@@ -1432,7 +2164,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!K1</f>
+              <f>'combined Stats-this session'!K1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1442,12 +2174,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$K$2:$K$6</f>
+              <f>'combined Stats-this session'!$K$2:$K$11</f>
             </numRef>
           </val>
         </ser>
@@ -1489,6 +2221,7 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -1514,7 +2247,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!O1</f>
+              <f>'combined Stats-this session'!O1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1524,12 +2257,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$O$2:$O$6</f>
+              <f>'combined Stats-this session'!$O$2:$O$11</f>
             </numRef>
           </val>
         </ser>
@@ -1538,7 +2271,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!P1</f>
+              <f>'combined Stats-this session'!P1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1548,12 +2281,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$P$2:$P$6</f>
+              <f>'combined Stats-this session'!$P$2:$P$11</f>
             </numRef>
           </val>
         </ser>
@@ -1598,6 +2331,7 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -1623,7 +2357,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!Q1</f>
+              <f>'combined Stats-this session'!Q1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1633,12 +2367,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$Q$2:$Q$6</f>
+              <f>'combined Stats-this session'!$Q$2:$Q$11</f>
             </numRef>
           </val>
         </ser>
@@ -1680,7 +2414,6 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -1808,7 +2541,6 @@
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -1891,7 +2623,6 @@
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="2"/>
   <chart>
     <title>
       <tx>
@@ -2008,7 +2739,7 @@
       <row>13</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7920000" cy="4464000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -2025,12 +2756,12 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>12</col>
+      <col>14</col>
       <colOff>0</colOff>
       <row>13</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7920000" cy="4464000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="2" name="Chart 2"/>
@@ -2052,7 +2783,7 @@
       <row>39</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7920000" cy="4464000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="3" name="Chart 3"/>
@@ -2069,12 +2800,12 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>12</col>
+      <col>14</col>
       <colOff>0</colOff>
       <row>39</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7920000" cy="4464000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="4" name="Chart 4"/>
@@ -2096,7 +2827,7 @@
       <row>65</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7920000" cy="4464000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="5" name="Chart 5"/>
@@ -2113,7 +2844,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>12</col>
+      <col>14</col>
       <colOff>0</colOff>
       <row>65</row>
       <rowOff>0</rowOff>
@@ -2145,7 +2876,7 @@
       <row>13</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7200000" cy="4031999"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -2162,12 +2893,12 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>12</col>
+      <col>14</col>
       <colOff>0</colOff>
       <row>13</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7200000" cy="4031999"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="2" name="Chart 2"/>
@@ -2189,7 +2920,7 @@
       <row>39</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7200000" cy="4031999"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="3" name="Chart 3"/>
@@ -2206,12 +2937,12 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>12</col>
+      <col>14</col>
       <colOff>0</colOff>
       <row>39</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7200000" cy="4031999"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="4" name="Chart 4"/>
@@ -2233,7 +2964,7 @@
       <row>65</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7200000" cy="4031999"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="5" name="Chart 5"/>
@@ -2250,7 +2981,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>12</col>
+      <col>14</col>
       <colOff>0</colOff>
       <row>65</row>
       <rowOff>0</rowOff>
@@ -2282,7 +3013,7 @@
       <row>13</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7200000" cy="4031999"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -2299,12 +3030,12 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>12</col>
+      <col>14</col>
       <colOff>0</colOff>
       <row>13</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7200000" cy="4031999"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="2" name="Chart 2"/>
@@ -2326,7 +3057,7 @@
       <row>39</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7200000" cy="4031999"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="3" name="Chart 3"/>
@@ -2343,12 +3074,12 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>12</col>
+      <col>14</col>
       <colOff>0</colOff>
       <row>39</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7200000" cy="4031999"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="4" name="Chart 4"/>
@@ -2370,7 +3101,7 @@
       <row>65</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="8640000" cy="4860000"/>
+    <ext cx="7200000" cy="4031999"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="5" name="Chart 5"/>
@@ -2387,7 +3118,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>12</col>
+      <col>14</col>
       <colOff>0</colOff>
       <row>65</row>
       <rowOff>0</rowOff>
@@ -2711,30 +3442,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="9.28515625" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
-    <col width="8.42578125" customWidth="1" style="3" min="2" max="2"/>
-    <col width="9.7109375" customWidth="1" style="3" min="3" max="3"/>
-    <col width="9.140625" customWidth="1" style="3" min="4" max="5"/>
-    <col width="6.28515625" customWidth="1" style="3" min="6" max="6"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="3" min="7" max="7"/>
-    <col width="9.85546875" bestFit="1" customWidth="1" style="3" min="8" max="8"/>
-    <col width="12" bestFit="1" customWidth="1" style="3" min="9" max="9"/>
-    <col width="16" bestFit="1" customWidth="1" style="3" min="10" max="10"/>
-    <col width="18.5703125" bestFit="1" customWidth="1" style="3" min="11" max="11"/>
-    <col width="17.7109375" bestFit="1" customWidth="1" style="3" min="12" max="12"/>
-    <col width="28.5703125" bestFit="1" customWidth="1" style="3" min="13" max="13"/>
-    <col width="24.140625" bestFit="1" customWidth="1" style="3" min="14" max="14"/>
-    <col width="16.5703125" customWidth="1" style="3" min="15" max="15"/>
-    <col width="19" customWidth="1" style="3" min="16" max="16"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -2779,7 +3493,7 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Aggro Factor</t>
+          <t>Aggression Factor</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -2822,292 +3536,564 @@
           <t>Hands played</t>
         </is>
       </c>
-      <c r="R1" s="8" t="n"/>
-      <c r="S1" s="8" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fish</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>-20</v>
+        <v>46.46</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6.46</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>0.632</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>0.018</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>0.136</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <v>0.135</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>0.067</v>
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.617</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>0.406</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0.0391</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>0.421</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>0.227</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>0.125</v>
       </c>
       <c r="L2" t="n">
-        <v>0.27</v>
+        <v>1.67</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="N2" t="n">
-        <v>5</v>
-      </c>
-      <c r="O2" s="6" t="n">
-        <v>63.76</v>
-      </c>
-      <c r="P2" s="7" t="n">
-        <v>40.99</v>
-      </c>
-      <c r="Q2" s="8" t="n">
-        <v>163</v>
+        <v>23</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>147</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>37.68</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Scott</t>
+          <t>Cedric</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>50.08</v>
+        <v>22.25</v>
       </c>
       <c r="D3" t="n">
-        <v>15.08</v>
+        <v>-7.75</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="5" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>0.459</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>0.06469999999999999</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>0.613</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <v>0.124</v>
-      </c>
-      <c r="K3" s="5" t="n">
-        <v>0.047</v>
+      <c r="F3" s="1" t="n">
+        <v>0.362</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>0.057</v>
       </c>
       <c r="L3" t="n">
-        <v>4.15</v>
+        <v>0.37</v>
       </c>
       <c r="M3" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>70</v>
-      </c>
-      <c r="O3" s="6" t="n">
-        <v>109.4</v>
-      </c>
-      <c r="P3" s="7" t="n">
-        <v>157.65</v>
-      </c>
-      <c r="Q3" s="8" t="n">
-        <v>170</v>
+        <v>5</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>48.54</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>8.15</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>141</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>0607</t>
+          <t>05/04</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Raymond</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C4" t="n">
-        <v>32.33</v>
+        <v>66.01000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>12.33</v>
+        <v>36.01</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0.324</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>0.147</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>0.0353</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>0.224</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>0.106</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>0.065</v>
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.648</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0.214</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0.097</v>
       </c>
       <c r="L4" t="n">
-        <v>1.15</v>
+        <v>0.52</v>
       </c>
       <c r="M4" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>24</v>
-      </c>
-      <c r="O4" s="6" t="n">
-        <v>61.34</v>
-      </c>
-      <c r="P4" s="6" t="n">
-        <v>66.23999999999999</v>
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>322.53</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>13.92</v>
       </c>
       <c r="Q4" t="n">
-        <v>170</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jonathan</t>
+          <t>Kynan</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>-40</v>
+      <c r="D5" t="n">
+        <v>-30</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0.371</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="J5" s="5" t="n">
-        <v>0.081</v>
-      </c>
-      <c r="K5" s="5" t="n">
-        <v>0.04</v>
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.636</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0.178</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0.078</v>
       </c>
       <c r="L5" t="n">
-        <v>0.12</v>
+        <v>0.25</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6" t="n">
-        <v>6.68</v>
-      </c>
-      <c r="P5" s="6" t="n">
-        <v>11.4</v>
+        <v>4</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>48.56</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>4.9</v>
       </c>
       <c r="Q5" t="n">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cedric</t>
+          <t>Jonathan</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>20</v>
       </c>
       <c r="C6" t="n">
-        <v>52.59</v>
+        <v>19.51</v>
       </c>
       <c r="D6" t="n">
-        <v>32.59</v>
+        <v>-0.49</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="J6" s="5" t="n">
-        <v>0.062</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>0.037</v>
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.488</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>0.07000000000000001</v>
       </c>
       <c r="L6" t="n">
-        <v>0.46</v>
+        <v>0.24</v>
       </c>
       <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>10.52</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>6.95</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Fish</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>30</v>
+      </c>
+      <c r="C7" t="n">
+        <v>185.77</v>
+      </c>
+      <c r="D7" t="n">
+        <v>155.77</v>
+      </c>
+      <c r="E7" t="n">
         <v>2</v>
       </c>
-      <c r="N6" t="n">
+      <c r="F7" s="1" t="n">
+        <v>0.717</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0.0207</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>0.269</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>0.138</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="6" t="n">
-        <v>55.78</v>
-      </c>
-      <c r="P6" s="6" t="n">
-        <v>82.09</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>160</v>
+      <c r="O7" s="2" t="n">
+        <v>393.14</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>13.71</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Jacob</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>20</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-20</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0.609</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>0.152</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="P8" s="2" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Marshall</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>147.59</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <v>38.07</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Regan</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>120</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-120</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0.646</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>0.281</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>0.07290000000000001</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>0.418</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="M10" t="n">
+        <v>8</v>
+      </c>
+      <c r="N10" t="n">
+        <v>14</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>121.03</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <v>49.87</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Cheyenne</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0.675</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M11" t="n">
+        <v>2</v>
+      </c>
+      <c r="N11" t="n">
+        <v>2</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>10.94</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -3120,31 +4106,11 @@
   </sheetPr>
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="10" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
-    <col width="6.7109375" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
-    <col width="7.85546875" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
-    <col width="6.85546875" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
-    <col width="7.7109375" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
-    <col width="6.140625" bestFit="1" customWidth="1" style="3" min="6" max="6"/>
-    <col width="14.28515625" bestFit="1" customWidth="1" style="3" min="7" max="7"/>
-    <col width="10" bestFit="1" customWidth="1" style="3" min="8" max="8"/>
-    <col width="12.28515625" bestFit="1" customWidth="1" style="3" min="9" max="9"/>
-    <col width="16.140625" bestFit="1" customWidth="1" style="3" min="10" max="10"/>
-    <col width="19.140625" bestFit="1" customWidth="1" style="3" min="11" max="11"/>
-    <col width="18.42578125" bestFit="1" customWidth="1" style="3" min="12" max="12"/>
-    <col width="6.85546875" bestFit="1" customWidth="1" style="3" min="13" max="13"/>
-    <col width="19.28515625" bestFit="1" customWidth="1" style="3" min="14" max="14"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="3" min="15" max="15"/>
-    <col width="24.85546875" bestFit="1" customWidth="1" style="3" min="16" max="16"/>
-    <col width="13.85546875" bestFit="1" customWidth="1" style="3" min="17" max="17"/>
-    <col width="4.7109375" bestFit="1" customWidth="1" style="3" min="20" max="20"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -3189,7 +4155,7 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Aggro Factor</t>
+          <t>Aggression Factor</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -3232,8 +4198,6 @@
           <t>Hands played</t>
         </is>
       </c>
-      <c r="R1" s="8" t="n"/>
-      <c r="S1" s="8" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3247,28 +4211,28 @@
       <c r="C2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" t="n">
         <v>-20</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="n">
+      <c r="G2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="J2" s="5" t="n">
+      <c r="J2" s="1" t="n">
         <v>0.667</v>
       </c>
-      <c r="K2" s="5" t="n">
+      <c r="K2" s="1" t="n">
         <v>0.333</v>
       </c>
       <c r="L2" t="n">
@@ -3280,13 +4244,13 @@
       <c r="N2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="6" t="n">
+      <c r="O2" s="2" t="n">
         <v>5.59</v>
       </c>
-      <c r="P2" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="4" t="n">
+      <c r="P2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
         <v>3</v>
       </c>
     </row>
@@ -3308,22 +4272,22 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="G3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5" t="n">
+      <c r="G3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
@@ -3335,13 +4299,13 @@
       <c r="N3" t="n">
         <v>0</v>
       </c>
-      <c r="O3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="4" t="n">
+      <c r="O3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>2</v>
       </c>
       <c r="T3" t="inlineStr">
@@ -3368,22 +4332,22 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.882</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="1" t="n">
         <v>0.647</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="1" t="n">
         <v>0.1176</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="1" t="n">
         <v>0.6879999999999999</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="J4" s="1" t="n">
         <v>0.118</v>
       </c>
-      <c r="K4" s="5" t="n">
+      <c r="K4" s="1" t="n">
         <v>0.059</v>
       </c>
       <c r="L4" t="n">
@@ -3395,10 +4359,10 @@
       <c r="N4" t="n">
         <v>7</v>
       </c>
-      <c r="O4" s="6" t="n">
+      <c r="O4" s="2" t="n">
         <v>5.59</v>
       </c>
-      <c r="P4" s="6" t="n">
+      <c r="P4" s="2" t="n">
         <v>13.6</v>
       </c>
       <c r="Q4" t="n">
@@ -3423,22 +4387,22 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="1" t="n">
         <v>0.765</v>
       </c>
-      <c r="G5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5" t="n">
+      <c r="G5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="n">
         <v>0.295</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="1" t="n">
         <v>0.118</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="1" t="n">
         <v>0.118</v>
       </c>
       <c r="L5" t="n">
@@ -3450,10 +4414,10 @@
       <c r="N5" t="n">
         <v>0</v>
       </c>
-      <c r="O5" s="6" t="n">
+      <c r="O5" s="2" t="n">
         <v>19.83</v>
       </c>
-      <c r="P5" s="6" t="n">
+      <c r="P5" s="2" t="n">
         <v>8.109999999999999</v>
       </c>
       <c r="Q5" t="n">
@@ -3461,8 +4425,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -3473,33 +4436,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N67" sqref="N67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="7.140625" bestFit="1" customWidth="1" style="3" min="1" max="2"/>
-    <col width="8.42578125" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
-    <col width="9.7109375" customWidth="1" style="3" min="4" max="4"/>
-    <col width="8.140625" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
-    <col width="7.42578125" customWidth="1" style="3" min="6" max="6"/>
-    <col width="15.140625" bestFit="1" customWidth="1" style="3" min="7" max="7"/>
-    <col width="10.7109375" bestFit="1" customWidth="1" style="3" min="8" max="8"/>
-    <col width="17.140625" bestFit="1" customWidth="1" style="3" min="9" max="9"/>
-    <col width="20.28515625" bestFit="1" customWidth="1" style="3" min="10" max="10"/>
-    <col width="19.5703125" bestFit="1" customWidth="1" style="3" min="11" max="11"/>
-    <col width="12.7109375" customWidth="1" style="3" min="12" max="12"/>
-    <col width="7.28515625" bestFit="1" customWidth="1" style="3" min="13" max="13"/>
-    <col width="20.5703125" bestFit="1" customWidth="1" style="3" min="14" max="14"/>
-    <col width="14.42578125" customWidth="1" style="3" min="15" max="15"/>
-    <col width="18" customWidth="1" style="3" min="16" max="16"/>
-    <col width="14.85546875" bestFit="1" customWidth="1" style="3" min="17" max="17"/>
-    <col width="10.7109375" customWidth="1" style="3" min="18" max="18"/>
-    <col width="4.42578125" bestFit="1" customWidth="1" style="3" min="32" max="32"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -3544,24 +4487,24 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>Aggression Factor</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>Aggro Frequency</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Went to showdown</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Won at showdown</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Aggro Factor</t>
-        </is>
-      </c>
       <c r="M1" t="inlineStr">
         <is>
           <t>C-bets</t>
@@ -3569,7 +4512,7 @@
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Opportunities</t>
+          <t>C-bet opportunities</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
@@ -3587,8 +4530,6 @@
           <t>Hands played</t>
         </is>
       </c>
-      <c r="R1" s="8" t="n"/>
-      <c r="S1" s="8" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3602,29 +4543,29 @@
       <c r="C2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" t="n">
         <v>-20</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="5" t="n">
-        <v>0.639</v>
-      </c>
-      <c r="G2" s="5" t="n">
+      <c r="F2" s="1" t="n">
+        <v>0.632</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>0.018</v>
       </c>
-      <c r="H2" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>0.138</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <v>0.145</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>0.07199999999999999</v>
+      <c r="H2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>0.136</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>0.067</v>
       </c>
       <c r="L2" t="n">
         <v>0.27</v>
@@ -3635,19 +4576,14 @@
       <c r="N2" t="n">
         <v>5</v>
       </c>
-      <c r="O2" s="6" t="n">
-        <v>69.34999999999999</v>
-      </c>
-      <c r="P2" s="6" t="n">
+      <c r="O2" s="2" t="n">
+        <v>63.76</v>
+      </c>
+      <c r="P2" s="2" t="n">
         <v>40.99</v>
       </c>
       <c r="Q2" t="n">
-        <v>166</v>
-      </c>
-      <c r="R2" s="8" t="n"/>
-      <c r="S2" s="2" t="n"/>
-      <c r="AF2" t="n">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3">
@@ -3662,32 +4598,32 @@
       <c r="C3" t="n">
         <v>50.08</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" t="n">
         <v>15.08</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="5" t="n">
-        <v>0.698</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>0.453</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>0.064</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>0.607</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <v>0.122</v>
-      </c>
-      <c r="K3" s="5" t="n">
+      <c r="F3" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.459</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.06469999999999999</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0.613</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="K3" s="1" t="n">
         <v>0.047</v>
       </c>
       <c r="L3" t="n">
-        <v>4.06</v>
+        <v>4.15</v>
       </c>
       <c r="M3" t="n">
         <v>45</v>
@@ -3695,24 +4631,19 @@
       <c r="N3" t="n">
         <v>70</v>
       </c>
-      <c r="O3" s="6" t="n">
+      <c r="O3" s="2" t="n">
         <v>109.4</v>
       </c>
-      <c r="P3" s="6" t="n">
+      <c r="P3" s="2" t="n">
         <v>157.65</v>
       </c>
       <c r="Q3" t="n">
-        <v>172</v>
-      </c>
-      <c r="R3" s="8" t="n"/>
-      <c r="S3" s="2" t="n"/>
+        <v>170</v>
+      </c>
       <c r="T3" t="inlineStr">
         <is>
           <t>0607</t>
         </is>
-      </c>
-      <c r="AF3" t="n">
-        <v>117</v>
       </c>
     </row>
     <row r="4">
@@ -3733,41 +4664,41 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="5" t="n">
-        <v>0.374</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>0.193</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>0.0428</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>0.279</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>0.107</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>0.064</v>
+      <c r="F4" s="1" t="n">
+        <v>0.324</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0.0353</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0.065</v>
       </c>
       <c r="L4" t="n">
-        <v>1.47</v>
+        <v>1.15</v>
       </c>
       <c r="M4" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="N4" t="n">
-        <v>31</v>
-      </c>
-      <c r="O4" s="6" t="n">
-        <v>66.93000000000001</v>
-      </c>
-      <c r="P4" s="6" t="n">
-        <v>79.84</v>
+        <v>24</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>61.34</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>66.23999999999999</v>
       </c>
       <c r="Q4" t="n">
-        <v>187</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5">
@@ -3788,22 +4719,22 @@
       <c r="E5" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="1" t="n">
         <v>0.371</v>
       </c>
-      <c r="G5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5" t="n">
+      <c r="G5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="n">
         <v>0.04</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="1" t="n">
         <v>0.081</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="1" t="n">
         <v>0.04</v>
       </c>
       <c r="L5" t="n">
@@ -3815,10 +4746,10 @@
       <c r="N5" t="n">
         <v>0</v>
       </c>
-      <c r="O5" s="6" t="n">
+      <c r="O5" s="2" t="n">
         <v>6.68</v>
       </c>
-      <c r="P5" s="6" t="n">
+      <c r="P5" s="2" t="n">
         <v>11.4</v>
       </c>
       <c r="Q5" t="n">
@@ -3843,26 +4774,26 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="5" t="n">
-        <v>0.412</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>0.011</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <v>0.179</v>
-      </c>
-      <c r="J6" s="5" t="n">
-        <v>0.068</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>0.045</v>
+      <c r="F6" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0.062</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>0.037</v>
       </c>
       <c r="L6" t="n">
-        <v>0.49</v>
+        <v>0.46</v>
       </c>
       <c r="M6" t="n">
         <v>2</v>
@@ -3870,19 +4801,18 @@
       <c r="N6" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="6" t="n">
-        <v>75.61</v>
-      </c>
-      <c r="P6" s="6" t="n">
-        <v>90.2</v>
+      <c r="O6" s="2" t="n">
+        <v>55.78</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>82.09</v>
       </c>
       <c r="Q6" t="n">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Preparing to write GUI
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -168,12 +168,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$11</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$F$2:$F$11</f>
+              <f>'combined Stats-this session'!$F$2:$F$5</f>
             </numRef>
           </val>
         </ser>
@@ -192,12 +192,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$11</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$G$2:$G$11</f>
+              <f>'combined Stats-this session'!$G$2:$G$5</f>
             </numRef>
           </val>
         </ser>
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$11</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$H$2:$H$11</f>
+              <f>'combined Stats-this session'!$H$2:$H$5</f>
             </numRef>
           </val>
         </ser>
@@ -1208,12 +1208,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$11</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$L$2:$L$11</f>
+              <f>'combined Stats-this session'!$L$2:$L$5</f>
             </numRef>
           </val>
         </ser>
@@ -1291,12 +1291,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$11</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$M$2:$M$11</f>
+              <f>'combined Stats-this session'!$M$2:$M$5</f>
             </numRef>
           </val>
         </ser>
@@ -1315,12 +1315,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$11</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$N$2:$N$11</f>
+              <f>'combined Stats-this session'!$N$2:$N$5</f>
             </numRef>
           </val>
         </ser>
@@ -1401,12 +1401,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$11</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$J$2:$J$11</f>
+              <f>'combined Stats-this session'!$J$2:$J$5</f>
             </numRef>
           </val>
         </ser>
@@ -1425,12 +1425,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$11</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$K$2:$K$11</f>
+              <f>'combined Stats-this session'!$K$2:$K$5</f>
             </numRef>
           </val>
         </ser>
@@ -1508,12 +1508,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$11</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$O$2:$O$11</f>
+              <f>'combined Stats-this session'!$O$2:$O$5</f>
             </numRef>
           </val>
         </ser>
@@ -1532,12 +1532,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$11</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$P$2:$P$11</f>
+              <f>'combined Stats-this session'!$P$2:$P$5</f>
             </numRef>
           </val>
         </ser>
@@ -1618,12 +1618,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$11</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$Q$2:$Q$11</f>
+              <f>'combined Stats-this session'!$Q$2:$Q$5</f>
             </numRef>
           </val>
         </ser>
@@ -2693,7 +2693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2791,56 +2791,56 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Scott</t>
+          <t>Raymond</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C2" t="n">
-        <v>46.46</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>6.46</v>
+        <v>-60</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0.617</v>
+        <v>0.587</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0.406</v>
+        <v>0.331</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0.0391</v>
+        <v>0.0407</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>0.421</v>
+        <v>0.444</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.227</v>
+        <v>0.174</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>0.125</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="L2" t="n">
-        <v>1.67</v>
+        <v>2.08</v>
       </c>
       <c r="M2" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="N2" t="n">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>147</v>
+        <v>109.46</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>37.68</v>
+        <v>93.31999999999999</v>
       </c>
       <c r="Q2" t="n">
-        <v>128</v>
+        <v>172</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -2855,497 +2855,167 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C3" t="n">
-        <v>22.25</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-7.75</v>
+        <v>-50</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.362</v>
+        <v>0.513</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>0.05</v>
+        <v>0.013</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0.131</v>
+        <v>0.23</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>0.106</v>
+        <v>0.173</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>0.057</v>
+        <v>0.103</v>
       </c>
       <c r="L3" t="n">
-        <v>0.37</v>
+        <v>0.57</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>48.54</v>
+        <v>80.69</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>8.15</v>
+        <v>47.72</v>
       </c>
       <c r="Q3" t="n">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>05/04</t>
+          <t>06/10</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>Fish</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C4" t="n">
-        <v>66.01000000000001</v>
+        <v>80.84</v>
       </c>
       <c r="D4" t="n">
-        <v>36.01</v>
+        <v>40.84</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0.648</v>
+        <v>0.676</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0.007</v>
+        <v>0.005</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0.24</v>
+        <v>0.161</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>0.214</v>
+        <v>0.198</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.097</v>
+        <v>0.077</v>
       </c>
       <c r="L4" t="n">
-        <v>0.52</v>
+        <v>0.28</v>
       </c>
       <c r="M4" t="n">
         <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>322.53</v>
+        <v>212.21</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>13.92</v>
+        <v>85.87</v>
       </c>
       <c r="Q4" t="n">
-        <v>145</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kynan</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C5" t="n">
+        <v>89.16</v>
+      </c>
+      <c r="D5" t="n">
+        <v>69.16</v>
+      </c>
+      <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
-        <v>-30</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2</v>
-      </c>
       <c r="F5" s="1" t="n">
-        <v>0.636</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>0.016</v>
+        <v>0.314</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>0</v>
+        <v>0.0254</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>0.131</v>
+        <v>0.483</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>0.178</v>
+        <v>0.127</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>0.078</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="L5" t="n">
-        <v>0.25</v>
+        <v>2.09</v>
       </c>
       <c r="M5" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="N5" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>48.56</v>
+        <v>143.51</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>4.9</v>
+        <v>108.51</v>
       </c>
       <c r="Q5" t="n">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Jonathan</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>20</v>
-      </c>
-      <c r="C6" t="n">
-        <v>19.51</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-0.49</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>0.488</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>0.023</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2" t="n">
-        <v>10.52</v>
-      </c>
-      <c r="P6" s="2" t="n">
-        <v>6.95</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Fish</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>30</v>
-      </c>
-      <c r="C7" t="n">
-        <v>185.77</v>
-      </c>
-      <c r="D7" t="n">
-        <v>155.77</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>0.717</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>0.055</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>0.0207</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>0.106</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>0.269</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <v>0.138</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="M7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" t="n">
-        <v>2</v>
-      </c>
-      <c r="O7" s="2" t="n">
-        <v>393.14</v>
-      </c>
-      <c r="P7" s="2" t="n">
-        <v>13.71</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Jacob</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>20</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-20</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>0.609</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>0.108</v>
-      </c>
-      <c r="J8" s="1" t="n">
-        <v>0.152</v>
-      </c>
-      <c r="K8" s="1" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2" t="n">
-        <v>48.5</v>
-      </c>
-      <c r="P8" s="2" t="n">
-        <v>18.2</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Marshall</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>10</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-10</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>0.673</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>0.029</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>0.134</v>
-      </c>
-      <c r="J9" s="1" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="K9" s="1" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>2</v>
-      </c>
-      <c r="O9" s="2" t="n">
-        <v>147.59</v>
-      </c>
-      <c r="P9" s="2" t="n">
-        <v>38.07</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Regan</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>120</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-120</v>
-      </c>
-      <c r="E10" t="n">
-        <v>4</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>0.646</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>0.281</v>
-      </c>
-      <c r="H10" s="1" t="n">
-        <v>0.07290000000000001</v>
-      </c>
-      <c r="I10" s="1" t="n">
-        <v>0.418</v>
-      </c>
-      <c r="J10" s="1" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="K10" s="1" t="n">
-        <v>0.094</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1.37</v>
-      </c>
-      <c r="M10" t="n">
-        <v>8</v>
-      </c>
-      <c r="N10" t="n">
-        <v>14</v>
-      </c>
-      <c r="O10" s="2" t="n">
-        <v>121.03</v>
-      </c>
-      <c r="P10" s="2" t="n">
-        <v>49.87</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Cheyenne</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>10</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>-10</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>0.675</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>0.122</v>
-      </c>
-      <c r="J11" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="K11" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="M11" t="n">
-        <v>2</v>
-      </c>
-      <c r="N11" t="n">
-        <v>2</v>
-      </c>
-      <c r="O11" s="2" t="n">
-        <v>10.94</v>
-      </c>
-      <c r="P11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>40</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed naming of columns
Column names were out of order. They are now corrected to show the correct stat in Excel.
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -4176,22 +4176,22 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>Aggro Frequency</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Went to showdown</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Won at showdown</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>Aggression Factor</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Aggro Frequency</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Went to showdown</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Won at showdown</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">

</xml_diff>

<commit_message>
Preparing to fix I/O issues
This commit is before I make the entire pokerStats.py script a function.
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -265,38 +265,27 @@
       <tx>
         <rich>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Went to showdown vs Won at showdown</a:t>
             </a:r>
           </a:p>
         </rich>
       </tx>
-      <overlay val="0"/>
     </title>
     <plotArea>
-      <layout/>
       <barChart>
         <barDir val="col"/>
         <grouping val="clustered"/>
-        <varyColors val="0"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!$J$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>Aggro Frequency</v>
-                </pt>
-              </strCache>
+              <f>'NL Stats-this session'!J1</f>
             </strRef>
           </tx>
           <spPr>
@@ -304,68 +293,14 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <invertIfNegative val="0"/>
-          <dLbls>
-            <spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-            <showLegendKey val="0"/>
-            <showVal val="1"/>
-            <showCatName val="0"/>
-            <showSerName val="0"/>
-            <showPercent val="0"/>
-            <showBubbleSize val="0"/>
-            <showLeaderLines val="0"/>
-          </dLbls>
           <cat>
-            <strRef>
+            <numRef>
               <f>'NL Stats-this session'!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Raymond</v>
-                </pt>
-                <pt idx="1">
-                  <v>Cedric</v>
-                </pt>
-                <pt idx="2">
-                  <v>Fish</v>
-                </pt>
-                <pt idx="3">
-                  <v>Scotty</v>
-                </pt>
-                <pt idx="4">
-                  <v>Regan</v>
-                </pt>
-              </strCache>
-            </strRef>
+            </numRef>
           </cat>
           <val>
             <numRef>
               <f>'NL Stats-this session'!$J$2:$J$6</f>
-              <numCache>
-                <formatCode>0.0%</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>0.137</v>
-                </pt>
-                <pt idx="1">
-                  <v>0.206</v>
-                </pt>
-                <pt idx="2">
-                  <v>0.267</v>
-                </pt>
-                <pt idx="3">
-                  <v>0.216</v>
-                </pt>
-                <pt idx="4">
-                  <v>0.167</v>
-                </pt>
-              </numCache>
             </numRef>
           </val>
         </ser>
@@ -374,13 +309,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!$K$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>Went to showdown</v>
-                </pt>
-              </strCache>
+              <f>'NL Stats-this session'!K1</f>
             </strRef>
           </tx>
           <spPr>
@@ -388,78 +317,19 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <invertIfNegative val="0"/>
-          <dLbls>
-            <spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-            <showLegendKey val="0"/>
-            <showVal val="1"/>
-            <showCatName val="0"/>
-            <showSerName val="0"/>
-            <showPercent val="0"/>
-            <showBubbleSize val="0"/>
-            <showLeaderLines val="0"/>
-          </dLbls>
           <cat>
-            <strRef>
+            <numRef>
               <f>'NL Stats-this session'!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Raymond</v>
-                </pt>
-                <pt idx="1">
-                  <v>Cedric</v>
-                </pt>
-                <pt idx="2">
-                  <v>Fish</v>
-                </pt>
-                <pt idx="3">
-                  <v>Scotty</v>
-                </pt>
-                <pt idx="4">
-                  <v>Regan</v>
-                </pt>
-              </strCache>
-            </strRef>
+            </numRef>
           </cat>
           <val>
             <numRef>
               <f>'NL Stats-this session'!$K$2:$K$6</f>
-              <numCache>
-                <formatCode>0.0%</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>0.054</v>
-                </pt>
-                <pt idx="1">
-                  <v>0.09</v>
-                </pt>
-                <pt idx="2">
-                  <v>0.186</v>
-                </pt>
-                <pt idx="3">
-                  <v>0.068</v>
-                </pt>
-                <pt idx="4">
-                  <v>0.028</v>
-                </pt>
-              </numCache>
             </numRef>
           </val>
         </ser>
         <dLbls>
-          <showLegendKey val="0"/>
           <showVal val="1"/>
-          <showCatName val="0"/>
-          <showSerName val="0"/>
-          <showPercent val="0"/>
-          <showBubbleSize val="0"/>
         </dLbls>
         <gapWidth val="150"/>
         <axId val="10"/>
@@ -470,34 +340,22 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
-        <axPos val="b"/>
-        <numFmt formatCode="General" sourceLinked="1"/>
+        <axPos val="l"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="100"/>
-        <crosses val="autoZero"/>
-        <auto val="0"/>
-        <lblAlgn val="ctr"/>
         <lblOffset val="100"/>
-        <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="0.0%" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="10"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="between"/>
       </valAx>
     </plotArea>
     <plotVisOnly val="1"/>
@@ -513,38 +371,27 @@
       <tx>
         <rich>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Money won</a:t>
             </a:r>
           </a:p>
         </rich>
       </tx>
-      <overlay val="0"/>
     </title>
     <plotArea>
-      <layout/>
       <barChart>
         <barDir val="col"/>
         <grouping val="clustered"/>
-        <varyColors val="0"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!$O$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>At showdown</v>
-                </pt>
-              </strCache>
+              <f>'NL Stats-this session'!O1</f>
             </strRef>
           </tx>
           <spPr>
@@ -552,68 +399,14 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <invertIfNegative val="0"/>
-          <dLbls>
-            <spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-            <showLegendKey val="0"/>
-            <showVal val="1"/>
-            <showCatName val="0"/>
-            <showSerName val="0"/>
-            <showPercent val="0"/>
-            <showBubbleSize val="0"/>
-            <showLeaderLines val="0"/>
-          </dLbls>
           <cat>
-            <strRef>
+            <numRef>
               <f>'NL Stats-this session'!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Raymond</v>
-                </pt>
-                <pt idx="1">
-                  <v>Cedric</v>
-                </pt>
-                <pt idx="2">
-                  <v>Fish</v>
-                </pt>
-                <pt idx="3">
-                  <v>Scotty</v>
-                </pt>
-                <pt idx="4">
-                  <v>Regan</v>
-                </pt>
-              </strCache>
-            </strRef>
+            </numRef>
           </cat>
           <val>
             <numRef>
               <f>'NL Stats-this session'!$O$2:$O$6</f>
-              <numCache>
-                <formatCode>"$"#,##0.00_-</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>74.34</v>
-                </pt>
-                <pt idx="1">
-                  <v>139.23</v>
-                </pt>
-                <pt idx="2">
-                  <v>250.58</v>
-                </pt>
-                <pt idx="3">
-                  <v>91.48999999999999</v>
-                </pt>
-                <pt idx="4">
-                  <v>42.6</v>
-                </pt>
-              </numCache>
             </numRef>
           </val>
         </ser>
@@ -622,13 +415,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!$P$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>Before showdown</v>
-                </pt>
-              </strCache>
+              <f>'NL Stats-this session'!P1</f>
             </strRef>
           </tx>
           <spPr>
@@ -636,78 +423,19 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <invertIfNegative val="0"/>
-          <dLbls>
-            <spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-            <showLegendKey val="0"/>
-            <showVal val="1"/>
-            <showCatName val="0"/>
-            <showSerName val="0"/>
-            <showPercent val="0"/>
-            <showBubbleSize val="0"/>
-            <showLeaderLines val="0"/>
-          </dLbls>
           <cat>
-            <strRef>
+            <numRef>
               <f>'NL Stats-this session'!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Raymond</v>
-                </pt>
-                <pt idx="1">
-                  <v>Cedric</v>
-                </pt>
-                <pt idx="2">
-                  <v>Fish</v>
-                </pt>
-                <pt idx="3">
-                  <v>Scotty</v>
-                </pt>
-                <pt idx="4">
-                  <v>Regan</v>
-                </pt>
-              </strCache>
-            </strRef>
+            </numRef>
           </cat>
           <val>
             <numRef>
               <f>'NL Stats-this session'!$P$2:$P$6</f>
-              <numCache>
-                <formatCode>"$"#,##0.00_-</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>85.73</v>
-                </pt>
-                <pt idx="1">
-                  <v>66.83</v>
-                </pt>
-                <pt idx="2">
-                  <v>28.54</v>
-                </pt>
-                <pt idx="3">
-                  <v>45.84</v>
-                </pt>
-                <pt idx="4">
-                  <v>27.8</v>
-                </pt>
-              </numCache>
             </numRef>
           </val>
         </ser>
         <dLbls>
-          <showLegendKey val="0"/>
           <showVal val="1"/>
-          <showCatName val="0"/>
-          <showSerName val="0"/>
-          <showPercent val="0"/>
-          <showBubbleSize val="0"/>
         </dLbls>
         <gapWidth val="150"/>
         <axId val="10"/>
@@ -718,39 +446,26 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
-        <axPos val="b"/>
-        <numFmt formatCode="General" sourceLinked="1"/>
+        <axPos val="l"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="100"/>
-        <crosses val="autoZero"/>
-        <auto val="0"/>
-        <lblAlgn val="ctr"/>
         <lblOffset val="100"/>
-        <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="&quot;$&quot;#,##0.00_-" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="10"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="between"/>
       </valAx>
     </plotArea>
     <legend>
       <legendPos val="b"/>
-      <overlay val="0"/>
     </legend>
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
@@ -765,38 +480,27 @@
       <tx>
         <rich>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Hands played</a:t>
             </a:r>
           </a:p>
         </rich>
       </tx>
-      <overlay val="0"/>
     </title>
     <plotArea>
-      <layout/>
       <barChart>
         <barDir val="bar"/>
         <grouping val="clustered"/>
-        <varyColors val="0"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!$Q$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>Hands played</v>
-                </pt>
-              </strCache>
+              <f>'NL Stats-this session'!Q1</f>
             </strRef>
           </tx>
           <spPr>
@@ -804,78 +508,19 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <invertIfNegative val="0"/>
-          <dLbls>
-            <spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-            <showLegendKey val="0"/>
-            <showVal val="1"/>
-            <showCatName val="0"/>
-            <showSerName val="0"/>
-            <showPercent val="0"/>
-            <showBubbleSize val="0"/>
-            <showLeaderLines val="0"/>
-          </dLbls>
           <cat>
-            <strRef>
+            <numRef>
               <f>'NL Stats-this session'!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Raymond</v>
-                </pt>
-                <pt idx="1">
-                  <v>Cedric</v>
-                </pt>
-                <pt idx="2">
-                  <v>Fish</v>
-                </pt>
-                <pt idx="3">
-                  <v>Scotty</v>
-                </pt>
-                <pt idx="4">
-                  <v>Regan</v>
-                </pt>
-              </strCache>
-            </strRef>
+            </numRef>
           </cat>
           <val>
             <numRef>
               <f>'NL Stats-this session'!$Q$2:$Q$6</f>
-              <numCache>
-                <formatCode>General</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>204</v>
-                </pt>
-                <pt idx="1">
-                  <v>199</v>
-                </pt>
-                <pt idx="2">
-                  <v>172</v>
-                </pt>
-                <pt idx="3">
-                  <v>74</v>
-                </pt>
-                <pt idx="4">
-                  <v>72</v>
-                </pt>
-              </numCache>
             </numRef>
           </val>
         </ser>
         <dLbls>
-          <showLegendKey val="0"/>
           <showVal val="1"/>
-          <showCatName val="0"/>
-          <showSerName val="0"/>
-          <showPercent val="0"/>
-          <showBubbleSize val="0"/>
         </dLbls>
         <gapWidth val="150"/>
         <axId val="10"/>
@@ -886,34 +531,22 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
         <axPos val="l"/>
-        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="100"/>
-        <crosses val="autoZero"/>
-        <auto val="0"/>
-        <lblAlgn val="ctr"/>
         <lblOffset val="100"/>
-        <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
-        <axPos val="b"/>
+        <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="10"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="between"/>
       </valAx>
     </plotArea>
     <plotVisOnly val="1"/>
@@ -2720,38 +2353,27 @@
       <tx>
         <rich>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>VPIP, Pre-flop raise, 3-bet</a:t>
             </a:r>
           </a:p>
         </rich>
       </tx>
-      <overlay val="0"/>
     </title>
     <plotArea>
-      <layout/>
       <barChart>
         <barDir val="col"/>
         <grouping val="clustered"/>
-        <varyColors val="0"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!$F$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>VPIP</v>
-                </pt>
-              </strCache>
+              <f>'NL Stats-this session'!F1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2759,52 +2381,14 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <invertIfNegative val="0"/>
           <cat>
-            <strRef>
+            <numRef>
               <f>'NL Stats-this session'!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Raymond</v>
-                </pt>
-                <pt idx="1">
-                  <v>Cedric</v>
-                </pt>
-                <pt idx="2">
-                  <v>Fish</v>
-                </pt>
-                <pt idx="3">
-                  <v>Scotty</v>
-                </pt>
-                <pt idx="4">
-                  <v>Regan</v>
-                </pt>
-              </strCache>
-            </strRef>
+            </numRef>
           </cat>
           <val>
             <numRef>
               <f>'NL Stats-this session'!$F$2:$F$6</f>
-              <numCache>
-                <formatCode>0.0%</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>0.475</v>
-                </pt>
-                <pt idx="1">
-                  <v>0.598</v>
-                </pt>
-                <pt idx="2">
-                  <v>0.657</v>
-                </pt>
-                <pt idx="3">
-                  <v>0.649</v>
-                </pt>
-                <pt idx="4">
-                  <v>0.514</v>
-                </pt>
-              </numCache>
             </numRef>
           </val>
         </ser>
@@ -2813,13 +2397,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!$G$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>Pre-flop Raise</v>
-                </pt>
-              </strCache>
+              <f>'NL Stats-this session'!G1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2827,52 +2405,14 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <invertIfNegative val="0"/>
           <cat>
-            <strRef>
+            <numRef>
               <f>'NL Stats-this session'!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Raymond</v>
-                </pt>
-                <pt idx="1">
-                  <v>Cedric</v>
-                </pt>
-                <pt idx="2">
-                  <v>Fish</v>
-                </pt>
-                <pt idx="3">
-                  <v>Scotty</v>
-                </pt>
-                <pt idx="4">
-                  <v>Regan</v>
-                </pt>
-              </strCache>
-            </strRef>
+            </numRef>
           </cat>
           <val>
             <numRef>
               <f>'NL Stats-this session'!$G$2:$G$6</f>
-              <numCache>
-                <formatCode>0.0%</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>0.27</v>
-                </pt>
-                <pt idx="1">
-                  <v>0.035</v>
-                </pt>
-                <pt idx="2">
-                  <v>0.006</v>
-                </pt>
-                <pt idx="3">
-                  <v>0.378</v>
-                </pt>
-                <pt idx="4">
-                  <v>0.194</v>
-                </pt>
-              </numCache>
             </numRef>
           </val>
         </ser>
@@ -2881,13 +2421,7 @@
           <order val="2"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!$H$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>Three-bet</v>
-                </pt>
-              </strCache>
+              <f>'NL Stats-this session'!H1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2895,63 +2429,17 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <invertIfNegative val="0"/>
           <cat>
-            <strRef>
+            <numRef>
               <f>'NL Stats-this session'!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Raymond</v>
-                </pt>
-                <pt idx="1">
-                  <v>Cedric</v>
-                </pt>
-                <pt idx="2">
-                  <v>Fish</v>
-                </pt>
-                <pt idx="3">
-                  <v>Scotty</v>
-                </pt>
-                <pt idx="4">
-                  <v>Regan</v>
-                </pt>
-              </strCache>
-            </strRef>
+            </numRef>
           </cat>
           <val>
             <numRef>
               <f>'NL Stats-this session'!$H$2:$H$6</f>
-              <numCache>
-                <formatCode>0.0%</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>0.0294</v>
-                </pt>
-                <pt idx="1">
-                  <v>0.005</v>
-                </pt>
-                <pt idx="2">
-                  <v>0</v>
-                </pt>
-                <pt idx="3">
-                  <v>0.08110000000000001</v>
-                </pt>
-                <pt idx="4">
-                  <v>0.0139</v>
-                </pt>
-              </numCache>
             </numRef>
           </val>
         </ser>
-        <dLbls>
-          <showLegendKey val="0"/>
-          <showVal val="0"/>
-          <showCatName val="0"/>
-          <showSerName val="0"/>
-          <showPercent val="0"/>
-          <showBubbleSize val="0"/>
-        </dLbls>
         <gapWidth val="150"/>
         <axId val="10"/>
         <axId val="100"/>
@@ -2961,34 +2449,22 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
-        <axPos val="b"/>
-        <numFmt formatCode="General" sourceLinked="1"/>
+        <axPos val="l"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="100"/>
-        <crosses val="autoZero"/>
-        <auto val="0"/>
-        <lblAlgn val="ctr"/>
         <lblOffset val="100"/>
-        <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="0.0%" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="10"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="between"/>
       </valAx>
     </plotArea>
     <plotVisOnly val="1"/>
@@ -3004,38 +2480,27 @@
       <tx>
         <rich>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Aggression Factor</a:t>
             </a:r>
           </a:p>
         </rich>
       </tx>
-      <overlay val="0"/>
     </title>
     <plotArea>
-      <layout/>
       <barChart>
         <barDir val="col"/>
         <grouping val="clustered"/>
-        <varyColors val="0"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!$L$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>Won at showdown</v>
-                </pt>
-              </strCache>
+              <f>'NL Stats-this session'!L1</f>
             </strRef>
           </tx>
           <spPr>
@@ -3043,78 +2508,19 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <invertIfNegative val="0"/>
-          <dLbls>
-            <spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-            <showLegendKey val="0"/>
-            <showVal val="1"/>
-            <showCatName val="0"/>
-            <showSerName val="0"/>
-            <showPercent val="0"/>
-            <showBubbleSize val="0"/>
-            <showLeaderLines val="0"/>
-          </dLbls>
           <cat>
-            <strRef>
+            <numRef>
               <f>'NL Stats-this session'!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Raymond</v>
-                </pt>
-                <pt idx="1">
-                  <v>Cedric</v>
-                </pt>
-                <pt idx="2">
-                  <v>Fish</v>
-                </pt>
-                <pt idx="3">
-                  <v>Scotty</v>
-                </pt>
-                <pt idx="4">
-                  <v>Regan</v>
-                </pt>
-              </strCache>
-            </strRef>
+            </numRef>
           </cat>
           <val>
             <numRef>
               <f>'NL Stats-this session'!$L$2:$L$6</f>
-              <numCache>
-                <formatCode>General</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>1.39</v>
-                </pt>
-                <pt idx="1">
-                  <v>0.55</v>
-                </pt>
-                <pt idx="2">
-                  <v>0.23</v>
-                </pt>
-                <pt idx="3">
-                  <v>4.37</v>
-                </pt>
-                <pt idx="4">
-                  <v>1.86</v>
-                </pt>
-              </numCache>
             </numRef>
           </val>
         </ser>
         <dLbls>
-          <showLegendKey val="0"/>
           <showVal val="1"/>
-          <showCatName val="0"/>
-          <showSerName val="0"/>
-          <showPercent val="0"/>
-          <showBubbleSize val="0"/>
         </dLbls>
         <gapWidth val="150"/>
         <axId val="10"/>
@@ -3125,34 +2531,22 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
-        <axPos val="b"/>
-        <numFmt formatCode="General" sourceLinked="1"/>
+        <axPos val="l"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="100"/>
-        <crosses val="autoZero"/>
-        <auto val="0"/>
-        <lblAlgn val="ctr"/>
         <lblOffset val="100"/>
-        <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="10"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="between"/>
       </valAx>
     </plotArea>
     <plotVisOnly val="1"/>
@@ -3168,38 +2562,27 @@
       <tx>
         <rich>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>C-bets vs opportunities</a:t>
             </a:r>
           </a:p>
         </rich>
       </tx>
-      <overlay val="0"/>
     </title>
     <plotArea>
-      <layout/>
       <barChart>
         <barDir val="col"/>
         <grouping val="clustered"/>
-        <varyColors val="0"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!$M$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>C-bets</v>
-                </pt>
-              </strCache>
+              <f>'NL Stats-this session'!M1</f>
             </strRef>
           </tx>
           <spPr>
@@ -3207,68 +2590,14 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <invertIfNegative val="0"/>
-          <dLbls>
-            <spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-            <showLegendKey val="0"/>
-            <showVal val="1"/>
-            <showCatName val="0"/>
-            <showSerName val="0"/>
-            <showPercent val="0"/>
-            <showBubbleSize val="0"/>
-            <showLeaderLines val="0"/>
-          </dLbls>
           <cat>
-            <strRef>
+            <numRef>
               <f>'NL Stats-this session'!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Raymond</v>
-                </pt>
-                <pt idx="1">
-                  <v>Cedric</v>
-                </pt>
-                <pt idx="2">
-                  <v>Fish</v>
-                </pt>
-                <pt idx="3">
-                  <v>Scotty</v>
-                </pt>
-                <pt idx="4">
-                  <v>Regan</v>
-                </pt>
-              </strCache>
-            </strRef>
+            </numRef>
           </cat>
           <val>
             <numRef>
               <f>'NL Stats-this session'!$M$2:$M$6</f>
-              <numCache>
-                <formatCode>General</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>18</v>
-                </pt>
-                <pt idx="1">
-                  <v>6</v>
-                </pt>
-                <pt idx="2">
-                  <v>0</v>
-                </pt>
-                <pt idx="3">
-                  <v>16</v>
-                </pt>
-                <pt idx="4">
-                  <v>8</v>
-                </pt>
-              </numCache>
             </numRef>
           </val>
         </ser>
@@ -3277,13 +2606,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!$N$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>C-bet opportunities</v>
-                </pt>
-              </strCache>
+              <f>'NL Stats-this session'!N1</f>
             </strRef>
           </tx>
           <spPr>
@@ -3291,78 +2614,19 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <invertIfNegative val="0"/>
-          <dLbls>
-            <spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-            <showLegendKey val="0"/>
-            <showVal val="1"/>
-            <showCatName val="0"/>
-            <showSerName val="0"/>
-            <showPercent val="0"/>
-            <showBubbleSize val="0"/>
-            <showLeaderLines val="0"/>
-          </dLbls>
           <cat>
-            <strRef>
+            <numRef>
               <f>'NL Stats-this session'!$A$2:$A$6</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Raymond</v>
-                </pt>
-                <pt idx="1">
-                  <v>Cedric</v>
-                </pt>
-                <pt idx="2">
-                  <v>Fish</v>
-                </pt>
-                <pt idx="3">
-                  <v>Scotty</v>
-                </pt>
-                <pt idx="4">
-                  <v>Regan</v>
-                </pt>
-              </strCache>
-            </strRef>
+            </numRef>
           </cat>
           <val>
             <numRef>
               <f>'NL Stats-this session'!$N$2:$N$6</f>
-              <numCache>
-                <formatCode>General</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>55</v>
-                </pt>
-                <pt idx="1">
-                  <v>8</v>
-                </pt>
-                <pt idx="2">
-                  <v>0</v>
-                </pt>
-                <pt idx="3">
-                  <v>33</v>
-                </pt>
-                <pt idx="4">
-                  <v>16</v>
-                </pt>
-              </numCache>
             </numRef>
           </val>
         </ser>
         <dLbls>
-          <showLegendKey val="0"/>
           <showVal val="1"/>
-          <showCatName val="0"/>
-          <showSerName val="0"/>
-          <showPercent val="0"/>
-          <showBubbleSize val="0"/>
         </dLbls>
         <gapWidth val="150"/>
         <axId val="10"/>
@@ -3373,39 +2637,26 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
-        <axPos val="b"/>
-        <numFmt formatCode="General" sourceLinked="1"/>
+        <axPos val="l"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="100"/>
-        <crosses val="autoZero"/>
-        <auto val="0"/>
-        <lblAlgn val="ctr"/>
         <lblOffset val="100"/>
-        <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="10"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="between"/>
       </valAx>
     </plotArea>
     <legend>
       <legendPos val="b"/>
-      <overlay val="0"/>
     </legend>
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
@@ -4519,14 +3770,11 @@
   </sheetPr>
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="17.28515625" customWidth="1" min="9" max="9"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -4571,22 +3819,22 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>Aggro Frequency</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Went to showdown</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Won at showdown</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>Aggression Factor</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Aggro Frequency</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Went to showdown</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Won at showdown</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
@@ -4793,7 +4041,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Scotty</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Resetting and adding on both supported
Before, only add ons would be captured by the program. Now, you can either reset the stack or add on to it, and the program will capture it. It will not, however, capture cash outs or an artificial decrease in stack.
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -7,8 +7,8 @@
   </bookViews>
   <sheets>
     <sheet name="combined Stats-this session" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="PLO Stats-this session" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="NL Stats-this session" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="NL Stats-this session" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PLO Stats-this session" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -168,12 +168,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$F$2:$F$3</f>
+              <f>'combined Stats-this session'!$F$2:$F$5</f>
             </numRef>
           </val>
         </ser>
@@ -192,12 +192,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$G$2:$G$3</f>
+              <f>'combined Stats-this session'!$G$2:$G$5</f>
             </numRef>
           </val>
         </ser>
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$H$2:$H$3</f>
+              <f>'combined Stats-this session'!$H$2:$H$5</f>
             </numRef>
           </val>
         </ser>
@@ -285,7 +285,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!M1</f>
+              <f>'NL Stats-this session'!M1</f>
             </strRef>
           </tx>
           <spPr>
@@ -295,12 +295,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$M$2:$M$3</f>
+              <f>'NL Stats-this session'!$M$2:$M$5</f>
             </numRef>
           </val>
         </ser>
@@ -309,7 +309,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!N1</f>
+              <f>'NL Stats-this session'!N1</f>
             </strRef>
           </tx>
           <spPr>
@@ -319,12 +319,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$N$2:$N$3</f>
+              <f>'NL Stats-this session'!$N$2:$N$5</f>
             </numRef>
           </val>
         </ser>
@@ -394,7 +394,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!J1</f>
+              <f>'NL Stats-this session'!J1</f>
             </strRef>
           </tx>
           <spPr>
@@ -404,12 +404,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$J$2:$J$3</f>
+              <f>'NL Stats-this session'!$J$2:$J$5</f>
             </numRef>
           </val>
         </ser>
@@ -418,7 +418,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!K1</f>
+              <f>'NL Stats-this session'!K1</f>
             </strRef>
           </tx>
           <spPr>
@@ -428,12 +428,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$K$2:$K$3</f>
+              <f>'NL Stats-this session'!$K$2:$K$5</f>
             </numRef>
           </val>
         </ser>
@@ -500,7 +500,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!R1</f>
+              <f>'NL Stats-this session'!R1</f>
             </strRef>
           </tx>
           <spPr>
@@ -510,12 +510,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$R$2:$R$3</f>
+              <f>'NL Stats-this session'!$R$2:$R$5</f>
             </numRef>
           </val>
         </ser>
@@ -582,7 +582,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!O1</f>
+              <f>'NL Stats-this session'!O1</f>
             </strRef>
           </tx>
           <spPr>
@@ -592,12 +592,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$O$2:$O$3</f>
+              <f>'NL Stats-this session'!$O$2:$O$5</f>
             </numRef>
           </val>
         </ser>
@@ -606,7 +606,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!P1</f>
+              <f>'NL Stats-this session'!P1</f>
             </strRef>
           </tx>
           <spPr>
@@ -616,12 +616,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$P$2:$P$3</f>
+              <f>'NL Stats-this session'!$P$2:$P$5</f>
             </numRef>
           </val>
         </ser>
@@ -691,7 +691,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!Q1</f>
+              <f>'NL Stats-this session'!Q1</f>
             </strRef>
           </tx>
           <spPr>
@@ -701,12 +701,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$Q$2:$Q$3</f>
+              <f>'NL Stats-this session'!$Q$2:$Q$5</f>
             </numRef>
           </val>
         </ser>
@@ -773,7 +773,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!F1</f>
+              <f>'PLO Stats-this session'!F1</f>
             </strRef>
           </tx>
           <spPr>
@@ -783,12 +783,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$F$2:$F$5</f>
+              <f>'PLO Stats-this session'!$F$2:$F$3</f>
             </numRef>
           </val>
         </ser>
@@ -797,7 +797,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!G1</f>
+              <f>'PLO Stats-this session'!G1</f>
             </strRef>
           </tx>
           <spPr>
@@ -807,12 +807,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$G$2:$G$5</f>
+              <f>'PLO Stats-this session'!$G$2:$G$3</f>
             </numRef>
           </val>
         </ser>
@@ -821,7 +821,7 @@
           <order val="2"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!H1</f>
+              <f>'PLO Stats-this session'!H1</f>
             </strRef>
           </tx>
           <spPr>
@@ -831,12 +831,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$H$2:$H$5</f>
+              <f>'PLO Stats-this session'!$H$2:$H$3</f>
             </numRef>
           </val>
         </ser>
@@ -900,7 +900,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!L1</f>
+              <f>'PLO Stats-this session'!L1</f>
             </strRef>
           </tx>
           <spPr>
@@ -910,12 +910,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$L$2:$L$5</f>
+              <f>'PLO Stats-this session'!$L$2:$L$3</f>
             </numRef>
           </val>
         </ser>
@@ -982,7 +982,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!M1</f>
+              <f>'PLO Stats-this session'!M1</f>
             </strRef>
           </tx>
           <spPr>
@@ -992,12 +992,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$M$2:$M$5</f>
+              <f>'PLO Stats-this session'!$M$2:$M$3</f>
             </numRef>
           </val>
         </ser>
@@ -1006,7 +1006,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!N1</f>
+              <f>'PLO Stats-this session'!N1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1016,12 +1016,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$N$2:$N$5</f>
+              <f>'PLO Stats-this session'!$N$2:$N$3</f>
             </numRef>
           </val>
         </ser>
@@ -1091,7 +1091,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!J1</f>
+              <f>'PLO Stats-this session'!J1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1101,12 +1101,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$J$2:$J$5</f>
+              <f>'PLO Stats-this session'!$J$2:$J$3</f>
             </numRef>
           </val>
         </ser>
@@ -1115,7 +1115,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!K1</f>
+              <f>'PLO Stats-this session'!K1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1125,12 +1125,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$K$2:$K$5</f>
+              <f>'PLO Stats-this session'!$K$2:$K$3</f>
             </numRef>
           </val>
         </ser>
@@ -1197,7 +1197,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!R1</f>
+              <f>'PLO Stats-this session'!R1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1207,12 +1207,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$R$2:$R$5</f>
+              <f>'PLO Stats-this session'!$R$2:$R$3</f>
             </numRef>
           </val>
         </ser>
@@ -1290,12 +1290,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$L$2:$L$3</f>
+              <f>'combined Stats-this session'!$L$2:$L$5</f>
             </numRef>
           </val>
         </ser>
@@ -1362,7 +1362,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!O1</f>
+              <f>'PLO Stats-this session'!O1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1372,12 +1372,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$O$2:$O$5</f>
+              <f>'PLO Stats-this session'!$O$2:$O$3</f>
             </numRef>
           </val>
         </ser>
@@ -1386,7 +1386,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!P1</f>
+              <f>'PLO Stats-this session'!P1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1396,12 +1396,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$P$2:$P$5</f>
+              <f>'PLO Stats-this session'!$P$2:$P$3</f>
             </numRef>
           </val>
         </ser>
@@ -1471,7 +1471,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!Q1</f>
+              <f>'PLO Stats-this session'!Q1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1481,12 +1481,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$Q$2:$Q$5</f>
+              <f>'PLO Stats-this session'!$Q$2:$Q$3</f>
             </numRef>
           </val>
         </ser>
@@ -1564,12 +1564,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$M$2:$M$3</f>
+              <f>'combined Stats-this session'!$M$2:$M$5</f>
             </numRef>
           </val>
         </ser>
@@ -1588,12 +1588,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$N$2:$N$3</f>
+              <f>'combined Stats-this session'!$N$2:$N$5</f>
             </numRef>
           </val>
         </ser>
@@ -1674,12 +1674,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$J$2:$J$3</f>
+              <f>'combined Stats-this session'!$J$2:$J$5</f>
             </numRef>
           </val>
         </ser>
@@ -1698,12 +1698,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$K$2:$K$3</f>
+              <f>'combined Stats-this session'!$K$2:$K$5</f>
             </numRef>
           </val>
         </ser>
@@ -1781,12 +1781,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$R$2:$R$3</f>
+              <f>'combined Stats-this session'!$R$2:$R$5</f>
             </numRef>
           </val>
         </ser>
@@ -1864,12 +1864,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$O$2:$O$3</f>
+              <f>'combined Stats-this session'!$O$2:$O$5</f>
             </numRef>
           </val>
         </ser>
@@ -1888,12 +1888,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$P$2:$P$3</f>
+              <f>'combined Stats-this session'!$P$2:$P$5</f>
             </numRef>
           </val>
         </ser>
@@ -1974,12 +1974,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$3</f>
+              <f>'combined Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$Q$2:$Q$3</f>
+              <f>'combined Stats-this session'!$Q$2:$Q$5</f>
             </numRef>
           </val>
         </ser>
@@ -2046,7 +2046,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!F1</f>
+              <f>'NL Stats-this session'!F1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2056,12 +2056,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$F$2:$F$3</f>
+              <f>'NL Stats-this session'!$F$2:$F$5</f>
             </numRef>
           </val>
         </ser>
@@ -2070,7 +2070,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!G1</f>
+              <f>'NL Stats-this session'!G1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2080,12 +2080,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$G$2:$G$3</f>
+              <f>'NL Stats-this session'!$G$2:$G$5</f>
             </numRef>
           </val>
         </ser>
@@ -2094,7 +2094,7 @@
           <order val="2"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!H1</f>
+              <f>'NL Stats-this session'!H1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2104,12 +2104,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$H$2:$H$3</f>
+              <f>'NL Stats-this session'!$H$2:$H$5</f>
             </numRef>
           </val>
         </ser>
@@ -2173,7 +2173,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!L1</f>
+              <f>'NL Stats-this session'!L1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2183,12 +2183,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$L$2:$L$3</f>
+              <f>'NL Stats-this session'!$L$2:$L$5</f>
             </numRef>
           </val>
         </ser>
@@ -3006,7 +3006,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3109,59 +3109,59 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Raymond</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>68.69</v>
       </c>
       <c r="C2" t="n">
-        <v>13.42</v>
+        <v>46.72</v>
       </c>
       <c r="D2" t="n">
-        <v>-6.58</v>
+        <v>-21.97</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0.768</v>
+        <v>0.574</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0.642</v>
+        <v>0.252</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0</v>
+        <v>0.0074</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>0.755</v>
+        <v>0.459</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.316</v>
+        <v>0.159</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>0.105</v>
+        <v>0.052</v>
       </c>
       <c r="L2" t="n">
-        <v>7.47</v>
+        <v>2.02</v>
       </c>
       <c r="M2" t="n">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="N2" t="n">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>46.36</v>
+        <v>152.38</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>27</v>
+        <v>108.09</v>
       </c>
       <c r="Q2" t="n">
-        <v>95</v>
+        <v>270</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>0.333</v>
+        <v>0.326</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -3172,64 +3172,180 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Fish</t>
+          <t>Raymond</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>28.85</v>
       </c>
       <c r="C3" t="n">
-        <v>16.58</v>
+        <v>35.63</v>
       </c>
       <c r="D3" t="n">
-        <v>6.58</v>
+        <v>6.78</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.737</v>
+        <v>0.438</v>
       </c>
       <c r="G3" s="1" t="n">
+        <v>0.251</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.0318</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0.396</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>0.074</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="M3" t="n">
+        <v>25</v>
+      </c>
+      <c r="N3" t="n">
+        <v>74</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>130.71</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>85.92</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>283</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>0.553</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>06/21/21</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cedric</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n">
+        <v>20.88</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="F4" s="1" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="n">
-        <v>0.185</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>0.316</v>
-      </c>
-      <c r="K3" s="1" t="n">
-        <v>0.221</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="M3" t="n">
+      <c r="I4" s="1" t="n">
+        <v>0.204</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>165.24</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>51.72</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>259</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>0.612</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Fish</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" t="n">
+        <v>34.31</v>
+      </c>
+      <c r="D5" t="n">
+        <v>14.31</v>
+      </c>
+      <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="N3" t="n">
+      <c r="F5" s="1" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="O3" s="2" t="n">
-        <v>64.12</v>
-      </c>
-      <c r="P3" s="2" t="n">
-        <v>22.4</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>95</v>
-      </c>
-      <c r="R3" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>06/15/21</t>
-        </is>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0.097</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0.213</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0.112</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>90.27</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>89</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>0.526</v>
       </c>
     </row>
   </sheetData>
@@ -3239,6 +3355,360 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Buy in</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Buy out</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Net</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Rebuys</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>VPIP</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Pre-flop Raise</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Three-bet</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Aggro Frequency</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Went to showdown</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Won at showdown</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Aggression Factor</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>C-bets</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>C-bet opportunities</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>At showdown</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Before showdown</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Hands played</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>WTSD (rel)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Scott</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>68.69</v>
+      </c>
+      <c r="C2" t="n">
+        <v>46.72</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-21.97</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.574</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>0.252</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0.0074</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>0.459</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>0.159</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="M2" t="n">
+        <v>22</v>
+      </c>
+      <c r="N2" t="n">
+        <v>44</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>152.38</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>108.09</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>270</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>0.326</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Raymond</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>28.85</v>
+      </c>
+      <c r="C3" t="n">
+        <v>35.63</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6.78</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0.438</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.251</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.0318</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0.396</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>0.074</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="M3" t="n">
+        <v>25</v>
+      </c>
+      <c r="N3" t="n">
+        <v>74</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>130.71</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>85.92</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>283</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>0.553</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>06/21/21</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cedric</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n">
+        <v>20.88</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0.204</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>165.24</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>51.72</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>259</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>0.612</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Fish</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" t="n">
+        <v>34.31</v>
+      </c>
+      <c r="D5" t="n">
+        <v>14.31</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0.097</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0.213</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0.112</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>90.27</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>89</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>0.526</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3474,358 +3944,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:T5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Player</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Buy in</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Buy out</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Net</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Rebuys</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>VPIP</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Pre-flop Raise</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Three-bet</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Aggro Frequency</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Went to showdown</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Won at showdown</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Aggression Factor</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>C-bets</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>C-bet opportunities</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>At showdown</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Before showdown</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Hands played</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>WTSD (rel)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Scott</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>68.69</v>
-      </c>
-      <c r="C2" t="n">
-        <v>46.72</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-21.97</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>0.574</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>0.252</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>0.0667</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>0.459</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>0.159</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>0.052</v>
-      </c>
-      <c r="L2" t="n">
-        <v>2.02</v>
-      </c>
-      <c r="M2" t="n">
-        <v>22</v>
-      </c>
-      <c r="N2" t="n">
-        <v>44</v>
-      </c>
-      <c r="O2" s="2" t="n">
-        <v>152.38</v>
-      </c>
-      <c r="P2" s="2" t="n">
-        <v>108.09</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>270</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>0.326</v>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Raymond</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>28.85</v>
-      </c>
-      <c r="C3" t="n">
-        <v>35.63</v>
-      </c>
-      <c r="D3" t="n">
-        <v>6.78</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>0.438</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>0.251</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>0.0883</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>0.396</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>0.134</v>
-      </c>
-      <c r="K3" s="1" t="n">
-        <v>0.074</v>
-      </c>
-      <c r="L3" t="n">
-        <v>2.56</v>
-      </c>
-      <c r="M3" t="n">
-        <v>25</v>
-      </c>
-      <c r="N3" t="n">
-        <v>74</v>
-      </c>
-      <c r="O3" s="2" t="n">
-        <v>130.71</v>
-      </c>
-      <c r="P3" s="2" t="n">
-        <v>85.92</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>283</v>
-      </c>
-      <c r="R3" s="1" t="n">
-        <v>0.553</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>06/21/21</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Cedric</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>20</v>
-      </c>
-      <c r="C4" t="n">
-        <v>20.88</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>0.448</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>0.204</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>0.189</v>
-      </c>
-      <c r="K4" s="1" t="n">
-        <v>0.116</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="M4" t="n">
-        <v>2</v>
-      </c>
-      <c r="N4" t="n">
-        <v>2</v>
-      </c>
-      <c r="O4" s="2" t="n">
-        <v>165.24</v>
-      </c>
-      <c r="P4" s="2" t="n">
-        <v>51.72</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>259</v>
-      </c>
-      <c r="R4" s="1" t="n">
-        <v>0.612</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Fish</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>20</v>
-      </c>
-      <c r="C5" t="n">
-        <v>34.31</v>
-      </c>
-      <c r="D5" t="n">
-        <v>14.31</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>0.652</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>0.097</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>0.213</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>0.112</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2" t="n">
-        <v>90.27</v>
-      </c>
-      <c r="P5" s="2" t="n">
-        <v>11.4</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>89</v>
-      </c>
-      <c r="R5" s="1" t="n">
-        <v>0.526</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
'Task completed successfully' added
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -3826,59 +3826,59 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Raymond</t>
+          <t>Fish</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>39.46</v>
       </c>
       <c r="C2" t="n">
-        <v>13.42</v>
+        <v>19.46</v>
       </c>
       <c r="D2" t="n">
-        <v>-6.58</v>
+        <v>-20</v>
       </c>
       <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.857</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>0</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>0.768</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>0.642</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>0.755</v>
+        <v>0.3</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.316</v>
+        <v>0.429</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>0.105</v>
+        <v>0.357</v>
       </c>
       <c r="L2" t="n">
-        <v>7.47</v>
+        <v>0.5</v>
       </c>
       <c r="M2" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>46.36</v>
+        <v>28.4</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>27</v>
+        <v>3.8</v>
       </c>
       <c r="Q2" t="n">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>0.333</v>
+        <v>0.833</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -3889,63 +3889,63 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Fish</t>
+          <t>Cedric</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>16.58</v>
+        <v>25.37</v>
       </c>
       <c r="D3" t="n">
-        <v>6.58</v>
+        <v>5.37</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.737</v>
+        <v>0.643</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>0</v>
+        <v>0.143</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0.185</v>
+        <v>0.483</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>0.316</v>
+        <v>0.429</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>0.221</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="L3" t="n">
-        <v>0.28</v>
+        <v>1.4</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>64.12</v>
+        <v>3.6</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>22.4</v>
+        <v>5</v>
       </c>
       <c r="Q3" t="n">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>0.7</v>
+        <v>0.167</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>06/15/21</t>
+          <t>05/27/21</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Errors are shown in GUI
Any error generated by pokerStats() will be output to GUI now, so user knows that program must be debugged without looking at command line output.
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -7,8 +7,8 @@
   </bookViews>
   <sheets>
     <sheet name="combined Stats-this session" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="NL Stats-this session" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="PLO Stats-this session" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="PLO Stats-this session" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="NL Stats-this session" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'NL Stats-this session'!$A$2:$A$5</definedName>
@@ -291,7 +291,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!M1</f>
+              <f>'PLO Stats-this session'!M1</f>
             </strRef>
           </tx>
           <spPr>
@@ -301,12 +301,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$M$2:$M$5</f>
+              <f>'PLO Stats-this session'!$M$2:$M$7</f>
             </numRef>
           </val>
         </ser>
@@ -315,7 +315,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!N1</f>
+              <f>'PLO Stats-this session'!N1</f>
             </strRef>
           </tx>
           <spPr>
@@ -325,12 +325,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$N$2:$N$5</f>
+              <f>'PLO Stats-this session'!$N$2:$N$7</f>
             </numRef>
           </val>
         </ser>
@@ -400,7 +400,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!J1</f>
+              <f>'PLO Stats-this session'!J1</f>
             </strRef>
           </tx>
           <spPr>
@@ -410,12 +410,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$J$2:$J$5</f>
+              <f>'PLO Stats-this session'!$J$2:$J$7</f>
             </numRef>
           </val>
         </ser>
@@ -424,7 +424,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!K1</f>
+              <f>'PLO Stats-this session'!K1</f>
             </strRef>
           </tx>
           <spPr>
@@ -434,12 +434,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$K$2:$K$5</f>
+              <f>'PLO Stats-this session'!$K$2:$K$7</f>
             </numRef>
           </val>
         </ser>
@@ -506,7 +506,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!R1</f>
+              <f>'PLO Stats-this session'!R1</f>
             </strRef>
           </tx>
           <spPr>
@@ -516,12 +516,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$R$2:$R$5</f>
+              <f>'PLO Stats-this session'!$R$2:$R$7</f>
             </numRef>
           </val>
         </ser>
@@ -588,7 +588,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!O1</f>
+              <f>'PLO Stats-this session'!O1</f>
             </strRef>
           </tx>
           <spPr>
@@ -598,12 +598,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$O$2:$O$5</f>
+              <f>'PLO Stats-this session'!$O$2:$O$7</f>
             </numRef>
           </val>
         </ser>
@@ -612,7 +612,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!P1</f>
+              <f>'PLO Stats-this session'!P1</f>
             </strRef>
           </tx>
           <spPr>
@@ -622,12 +622,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$P$2:$P$5</f>
+              <f>'PLO Stats-this session'!$P$2:$P$7</f>
             </numRef>
           </val>
         </ser>
@@ -698,7 +698,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!Q1</f>
+              <f>'PLO Stats-this session'!Q1</f>
             </strRef>
           </tx>
           <spPr>
@@ -708,12 +708,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$Q$2:$Q$5</f>
+              <f>'PLO Stats-this session'!$Q$2:$Q$7</f>
             </numRef>
           </val>
         </ser>
@@ -780,7 +780,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!F1</f>
+              <f>'NL Stats-this session'!F1</f>
             </strRef>
           </tx>
           <spPr>
@@ -790,12 +790,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$F$2:$F$3</f>
+              <f>'NL Stats-this session'!$F$2:$F$8</f>
             </numRef>
           </val>
         </ser>
@@ -804,7 +804,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!G1</f>
+              <f>'NL Stats-this session'!G1</f>
             </strRef>
           </tx>
           <spPr>
@@ -814,12 +814,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$G$2:$G$3</f>
+              <f>'NL Stats-this session'!$G$2:$G$8</f>
             </numRef>
           </val>
         </ser>
@@ -828,7 +828,7 @@
           <order val="2"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!H1</f>
+              <f>'NL Stats-this session'!H1</f>
             </strRef>
           </tx>
           <spPr>
@@ -838,12 +838,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$H$2:$H$3</f>
+              <f>'NL Stats-this session'!$H$2:$H$8</f>
             </numRef>
           </val>
         </ser>
@@ -907,7 +907,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!L1</f>
+              <f>'NL Stats-this session'!L1</f>
             </strRef>
           </tx>
           <spPr>
@@ -917,12 +917,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$L$2:$L$3</f>
+              <f>'NL Stats-this session'!$L$2:$L$8</f>
             </numRef>
           </val>
         </ser>
@@ -989,7 +989,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!M1</f>
+              <f>'NL Stats-this session'!M1</f>
             </strRef>
           </tx>
           <spPr>
@@ -999,12 +999,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$M$2:$M$3</f>
+              <f>'NL Stats-this session'!$M$2:$M$8</f>
             </numRef>
           </val>
         </ser>
@@ -1013,7 +1013,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!N1</f>
+              <f>'NL Stats-this session'!N1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1023,12 +1023,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$N$2:$N$3</f>
+              <f>'NL Stats-this session'!$N$2:$N$8</f>
             </numRef>
           </val>
         </ser>
@@ -1098,7 +1098,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!J1</f>
+              <f>'NL Stats-this session'!J1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1108,12 +1108,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$J$2:$J$3</f>
+              <f>'NL Stats-this session'!$J$2:$J$8</f>
             </numRef>
           </val>
         </ser>
@@ -1122,7 +1122,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!K1</f>
+              <f>'NL Stats-this session'!K1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1132,12 +1132,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$K$2:$K$3</f>
+              <f>'NL Stats-this session'!$K$2:$K$8</f>
             </numRef>
           </val>
         </ser>
@@ -1204,7 +1204,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!R1</f>
+              <f>'NL Stats-this session'!R1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1214,12 +1214,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$R$2:$R$3</f>
+              <f>'NL Stats-this session'!$R$2:$R$8</f>
             </numRef>
           </val>
         </ser>
@@ -1369,7 +1369,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!O1</f>
+              <f>'NL Stats-this session'!O1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1379,12 +1379,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$O$2:$O$3</f>
+              <f>'NL Stats-this session'!$O$2:$O$8</f>
             </numRef>
           </val>
         </ser>
@@ -1393,7 +1393,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!P1</f>
+              <f>'NL Stats-this session'!P1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1403,12 +1403,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$P$2:$P$3</f>
+              <f>'NL Stats-this session'!$P$2:$P$8</f>
             </numRef>
           </val>
         </ser>
@@ -1479,7 +1479,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'PLO Stats-this session'!Q1</f>
+              <f>'NL Stats-this session'!Q1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1489,12 +1489,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$3</f>
+              <f>'NL Stats-this session'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$Q$2:$Q$3</f>
+              <f>'NL Stats-this session'!$Q$2:$Q$8</f>
             </numRef>
           </val>
         </ser>
@@ -2055,7 +2055,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!F1</f>
+              <f>'PLO Stats-this session'!F1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2065,12 +2065,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$F$2:$F$5</f>
+              <f>'PLO Stats-this session'!$F$2:$F$7</f>
             </numRef>
           </val>
         </ser>
@@ -2079,7 +2079,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!G1</f>
+              <f>'PLO Stats-this session'!G1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2089,12 +2089,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$G$2:$G$5</f>
+              <f>'PLO Stats-this session'!$G$2:$G$7</f>
             </numRef>
           </val>
         </ser>
@@ -2103,7 +2103,7 @@
           <order val="2"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!H1</f>
+              <f>'PLO Stats-this session'!H1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2113,12 +2113,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$H$2:$H$5</f>
+              <f>'PLO Stats-this session'!$H$2:$H$7</f>
             </numRef>
           </val>
         </ser>
@@ -2182,7 +2182,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'NL Stats-this session'!L1</f>
+              <f>'PLO Stats-this session'!L1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2192,12 +2192,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$5</f>
+              <f>'PLO Stats-this session'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$L$2:$L$5</f>
+              <f>'PLO Stats-this session'!$L$2:$L$7</f>
             </numRef>
           </val>
         </ser>
@@ -3369,7 +3369,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3479,52 +3479,52 @@
         <v>30</v>
       </c>
       <c r="C2" t="n">
-        <v>32.74</v>
+        <v>22.79</v>
       </c>
       <c r="D2" t="n">
-        <v>2.74</v>
+        <v>-7.21</v>
       </c>
       <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.761</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>0.609</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>0.539</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>0.353</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>0.0086</v>
-      </c>
       <c r="I2" s="1" t="n">
-        <v>0.503</v>
+        <v>0.534</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.203</v>
+        <v>0.261</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>0.073</v>
+        <v>0.109</v>
       </c>
       <c r="L2" t="n">
-        <v>3.16</v>
+        <v>3.06</v>
       </c>
       <c r="M2" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="N2" t="n">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>69.91</v>
+        <v>44.39</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>74.25</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="Q2" t="n">
-        <v>232</v>
+        <v>46</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>0.362</v>
+        <v>0.417</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -3535,180 +3535,296 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cedric</t>
+          <t>Fish</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>26.87</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>6.87</v>
+        <v>-30</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.466</v>
+        <v>0.84</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.173</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>0</v>
+        <v>0.09329999999999999</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0.175</v>
+        <v>0.141</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>0.203</v>
+        <v>0.347</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>0.129</v>
+        <v>0.147</v>
       </c>
       <c r="L3" t="n">
-        <v>0.41</v>
+        <v>0.23</v>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N3" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>92.98999999999999</v>
+        <v>59.15</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>35.3</v>
+        <v>7.42</v>
       </c>
       <c r="Q3" t="n">
-        <v>232</v>
+        <v>75</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>0.638</v>
+        <v>0.423</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>06/28/21</t>
+          <t>04/29/21</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Fish</t>
+          <t>Cedric</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C4" t="n">
-        <v>9.32</v>
+        <v>20.11</v>
       </c>
       <c r="D4" t="n">
-        <v>-10.68</v>
+        <v>-9.890000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0.504</v>
+        <v>0.584</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0</v>
+        <v>0.112</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>0</v>
+        <v>0.0112</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0.173</v>
+        <v>0.314</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>0.209</v>
+        <v>0.303</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.093</v>
+        <v>0.124</v>
       </c>
       <c r="L4" t="n">
-        <v>0.37</v>
+        <v>0.75</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>23.5</v>
+        <v>67.14</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>37.24</v>
+        <v>21</v>
       </c>
       <c r="Q4" t="n">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0.444</v>
+        <v>0.407</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Scott</t>
+          <t>Kynan</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>21.07</v>
+        <v>42.17</v>
       </c>
       <c r="D5" t="n">
-        <v>1.07</v>
+        <v>32.17</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>0.468</v>
+        <v>0.911</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>0.247</v>
+        <v>0.067</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>0.0519</v>
+        <v>0.0111</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>0.434</v>
+        <v>0.286</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>0.143</v>
+        <v>0.4</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>0.065</v>
+        <v>0.244</v>
       </c>
       <c r="L5" t="n">
-        <v>3.54</v>
+        <v>0.53</v>
       </c>
       <c r="M5" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="N5" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>31.58</v>
+        <v>176.88</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>17.6</v>
+        <v>19.94</v>
       </c>
       <c r="Q5" t="n">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="R5" s="1" t="n">
-        <v>0.455</v>
+        <v>0.611</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Jacob</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C6" t="n">
+        <v>32.22</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.877</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0.0137</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0.139</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0.342</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>0.151</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>108.45</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>73</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Scott</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>20</v>
+      </c>
+      <c r="C7" t="n">
+        <v>32.71</v>
+      </c>
+      <c r="D7" t="n">
+        <v>12.71</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0.592</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>0.294</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>0.204</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="M7" t="n">
+        <v>3</v>
+      </c>
+      <c r="N7" t="n">
+        <v>7</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>62.4</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>49</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -3723,7 +3839,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3826,59 +3942,59 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fish</t>
+          <t>Raymond</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>39.46</v>
+        <v>20</v>
       </c>
       <c r="C2" t="n">
-        <v>19.46</v>
+        <v>13.15</v>
       </c>
       <c r="D2" t="n">
-        <v>-20</v>
+        <v>-6.85</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0.857</v>
+        <v>0.262</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>0.3</v>
+        <v>0.176</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.429</v>
+        <v>0.103</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>0.357</v>
+        <v>0.065</v>
       </c>
       <c r="L2" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>28.4</v>
+        <v>61.7</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>3.8</v>
+        <v>6.93</v>
       </c>
       <c r="Q2" t="n">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>0.833</v>
+        <v>0.636</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -3889,64 +4005,354 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Regan</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>60</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-60</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0.282</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="M3" t="n">
+        <v>8</v>
+      </c>
+      <c r="N3" t="n">
+        <v>14</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>29.35</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>100</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>0.467</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>05/24/21</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Cedric</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B4" t="n">
         <v>20</v>
       </c>
-      <c r="C3" t="n">
-        <v>25.37</v>
-      </c>
-      <c r="D3" t="n">
-        <v>5.37</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="C4" t="n">
+        <v>89.54000000000001</v>
+      </c>
+      <c r="D4" t="n">
+        <v>69.54000000000001</v>
+      </c>
+      <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>0.643</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>0.143</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="F4" s="1" t="n">
+        <v>0.346</v>
+      </c>
+      <c r="G4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="n">
-        <v>0.483</v>
-      </c>
-      <c r="J3" s="1" t="n">
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0.129</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0.154</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>37.47</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>104</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>0.438</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Fish</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-40</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.721</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0.146</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0.269</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>88.22</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>18.44</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>104</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>0.464</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cheyenne</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>20</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-20</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="n">
         <v>0.429</v>
       </c>
-      <c r="K3" s="1" t="n">
-        <v>0.07099999999999999</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="M3" t="n">
-        <v>6</v>
-      </c>
-      <c r="N3" t="n">
-        <v>10</v>
-      </c>
-      <c r="O3" s="2" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="P3" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>14</v>
-      </c>
-      <c r="R3" s="1" t="n">
-        <v>0.167</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>05/27/21</t>
-        </is>
+      <c r="G6" s="1" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0.0119</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>11.38</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>84</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Scott</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>20</v>
+      </c>
+      <c r="C7" t="n">
+        <v>110.15</v>
+      </c>
+      <c r="D7" t="n">
+        <v>90.15000000000001</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0.634</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0.394</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0.0141</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>0.5669999999999999</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>0.183</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="L7" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="M7" t="n">
+        <v>18</v>
+      </c>
+      <c r="N7" t="n">
+        <v>27</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>112.97</v>
+      </c>
+      <c r="P7" s="2" t="n">
+        <v>62.11</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>71</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>0.615</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Jacob</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>50</v>
+      </c>
+      <c r="C8" t="n">
+        <v>17.16</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-32.84</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>17</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logs can either run as-is or reversed
PokerNow exports logs in ascending order (latest is at the top). The program can now handle this order, instead of having to reverse the order every time. However, a hard-coded exceptions list is available to read logs in descending order. This is for debugging purposes, as it is much easier to read the logs in descending order.
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -790,12 +790,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$F$2:$F$7</f>
+              <f>'PLO Stats-this session'!$F$2:$F$5</f>
             </numRef>
           </val>
         </ser>
@@ -814,12 +814,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$G$2:$G$7</f>
+              <f>'PLO Stats-this session'!$G$2:$G$5</f>
             </numRef>
           </val>
         </ser>
@@ -838,12 +838,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$H$2:$H$7</f>
+              <f>'PLO Stats-this session'!$H$2:$H$5</f>
             </numRef>
           </val>
         </ser>
@@ -917,12 +917,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$L$2:$L$7</f>
+              <f>'PLO Stats-this session'!$L$2:$L$5</f>
             </numRef>
           </val>
         </ser>
@@ -999,12 +999,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$M$2:$M$7</f>
+              <f>'PLO Stats-this session'!$M$2:$M$5</f>
             </numRef>
           </val>
         </ser>
@@ -1023,12 +1023,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$N$2:$N$7</f>
+              <f>'PLO Stats-this session'!$N$2:$N$5</f>
             </numRef>
           </val>
         </ser>
@@ -1108,12 +1108,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$J$2:$J$7</f>
+              <f>'PLO Stats-this session'!$J$2:$J$5</f>
             </numRef>
           </val>
         </ser>
@@ -1132,12 +1132,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$K$2:$K$7</f>
+              <f>'PLO Stats-this session'!$K$2:$K$5</f>
             </numRef>
           </val>
         </ser>
@@ -1214,12 +1214,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$R$2:$R$7</f>
+              <f>'PLO Stats-this session'!$R$2:$R$5</f>
             </numRef>
           </val>
         </ser>
@@ -1379,12 +1379,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$O$2:$O$7</f>
+              <f>'PLO Stats-this session'!$O$2:$O$5</f>
             </numRef>
           </val>
         </ser>
@@ -1403,12 +1403,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$P$2:$P$7</f>
+              <f>'PLO Stats-this session'!$P$2:$P$5</f>
             </numRef>
           </val>
         </ser>
@@ -1489,12 +1489,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'PLO Stats-this session'!$A$2:$A$7</f>
+              <f>'PLO Stats-this session'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'PLO Stats-this session'!$Q$2:$Q$7</f>
+              <f>'PLO Stats-this session'!$Q$2:$Q$5</f>
             </numRef>
           </val>
         </ser>
@@ -3723,7 +3723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3830,55 +3830,55 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C2" t="n">
-        <v>22.79</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-7.21</v>
+        <v>-60</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0.761</v>
+        <v>0.713</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0.609</v>
+        <v>0.438</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>0.534</v>
+        <v>0.497</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.261</v>
+        <v>0.175</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>0.109</v>
+        <v>0.075</v>
       </c>
       <c r="L2" t="n">
-        <v>3.06</v>
+        <v>2.31</v>
       </c>
       <c r="M2" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="N2" t="n">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>44.39</v>
+        <v>72.64</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>9.369999999999999</v>
+        <v>59.64</v>
       </c>
       <c r="Q2" t="n">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>0.417</v>
+        <v>0.429</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -3889,296 +3889,180 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Fish</t>
+          <t>Cedric</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-30</v>
+        <v>-50</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.84</v>
+        <v>0.614</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>0.173</v>
+        <v>0.014</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>0.09329999999999999</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0.141</v>
+        <v>0.268</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>0.347</v>
+        <v>0.2</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>0.147</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="L3" t="n">
-        <v>0.23</v>
+        <v>0.6</v>
       </c>
       <c r="M3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>59.15</v>
+        <v>29.45</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>7.42</v>
+        <v>36.72</v>
       </c>
       <c r="Q3" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>0.423</v>
+        <v>0.429</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>04/29/21</t>
+          <t>06/10/21</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cedric</t>
+          <t>Fish</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C4" t="n">
-        <v>20.11</v>
+        <v>80.84</v>
       </c>
       <c r="D4" t="n">
-        <v>-9.890000000000001</v>
+        <v>40.84</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0.584</v>
+        <v>0.772</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0.112</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>0.0112</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0.314</v>
+        <v>0.171</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>0.303</v>
+        <v>0.207</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.124</v>
+        <v>0.098</v>
       </c>
       <c r="L4" t="n">
-        <v>0.75</v>
+        <v>0.29</v>
       </c>
       <c r="M4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>67.14</v>
+        <v>175.94</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>21</v>
+        <v>51.3</v>
       </c>
       <c r="Q4" t="n">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0.407</v>
+        <v>0.474</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kynan</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C5" t="n">
-        <v>42.17</v>
+        <v>89.16</v>
       </c>
       <c r="D5" t="n">
-        <v>32.17</v>
+        <v>69.16</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>0.911</v>
+        <v>0.788</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>0.067</v>
+        <v>0.288</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>0.0111</v>
+        <v>0.0192</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>0.286</v>
+        <v>0.45</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>0.4</v>
+        <v>0.173</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>0.244</v>
+        <v>0.115</v>
       </c>
       <c r="L5" t="n">
-        <v>0.53</v>
+        <v>1.5</v>
       </c>
       <c r="M5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N5" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>176.88</v>
+        <v>117.77</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>19.94</v>
+        <v>37.59</v>
       </c>
       <c r="Q5" t="n">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="R5" s="1" t="n">
-        <v>0.611</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Jacob</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>30</v>
-      </c>
-      <c r="C6" t="n">
-        <v>32.22</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>0.877</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>0.014</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>0.0137</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>0.139</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>0.342</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>0.151</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2" t="n">
-        <v>108.45</v>
-      </c>
-      <c r="P6" s="2" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>73</v>
-      </c>
-      <c r="R6" s="1" t="n">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Scott</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>20</v>
-      </c>
-      <c r="C7" t="n">
-        <v>32.71</v>
-      </c>
-      <c r="D7" t="n">
-        <v>12.71</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>0.592</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>0.122</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>0.294</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>0.204</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <v>0.082</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="M7" t="n">
-        <v>3</v>
-      </c>
-      <c r="N7" t="n">
-        <v>7</v>
-      </c>
-      <c r="O7" s="2" t="n">
-        <v>62.4</v>
-      </c>
-      <c r="P7" s="2" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>49</v>
-      </c>
-      <c r="R7" s="1" t="n">
-        <v>0.4</v>
+        <v>0.667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made to GUI
Added icon photo to GUI. Also, added buttons to GUI to directly open some Excel spreadsheets. Will be easy to add more as well, to open any document, using `os.system('path')`.
</commit_message>
<xml_diff>
--- a/Outputs/stats.xlsx
+++ b/Outputs/stats.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="combined Stats-this session" sheetId="1" state="visible" r:id="rId1"/>
@@ -167,12 +167,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$F$2:$F$6</f>
+              <f>'combined Stats-this session'!$F$2:$F$4</f>
             </numRef>
           </val>
         </ser>
@@ -191,12 +191,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$G$2:$G$6</f>
+              <f>'combined Stats-this session'!$G$2:$G$4</f>
             </numRef>
           </val>
         </ser>
@@ -215,12 +215,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$H$2:$H$6</f>
+              <f>'combined Stats-this session'!$H$2:$H$4</f>
             </numRef>
           </val>
         </ser>
@@ -294,12 +294,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$M$2:$M$6</f>
+              <f>'NL Stats-this session'!$M$2:$M$4</f>
             </numRef>
           </val>
         </ser>
@@ -318,12 +318,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$N$2:$N$6</f>
+              <f>'NL Stats-this session'!$N$2:$N$4</f>
             </numRef>
           </val>
         </ser>
@@ -403,12 +403,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$J$2:$J$6</f>
+              <f>'NL Stats-this session'!$J$2:$J$4</f>
             </numRef>
           </val>
         </ser>
@@ -427,12 +427,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$K$2:$K$6</f>
+              <f>'NL Stats-this session'!$K$2:$K$4</f>
             </numRef>
           </val>
         </ser>
@@ -509,12 +509,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$R$2:$R$6</f>
+              <f>'NL Stats-this session'!$R$2:$R$4</f>
             </numRef>
           </val>
         </ser>
@@ -591,12 +591,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$O$2:$O$6</f>
+              <f>'NL Stats-this session'!$O$2:$O$4</f>
             </numRef>
           </val>
         </ser>
@@ -615,12 +615,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$P$2:$P$6</f>
+              <f>'NL Stats-this session'!$P$2:$P$4</f>
             </numRef>
           </val>
         </ser>
@@ -701,12 +701,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$Q$2:$Q$6</f>
+              <f>'NL Stats-this session'!$Q$2:$Q$4</f>
             </numRef>
           </val>
         </ser>
@@ -784,12 +784,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$L$2:$L$6</f>
+              <f>'combined Stats-this session'!$L$2:$L$4</f>
             </numRef>
           </val>
         </ser>
@@ -867,12 +867,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$M$2:$M$6</f>
+              <f>'combined Stats-this session'!$M$2:$M$4</f>
             </numRef>
           </val>
         </ser>
@@ -891,12 +891,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$N$2:$N$6</f>
+              <f>'combined Stats-this session'!$N$2:$N$4</f>
             </numRef>
           </val>
         </ser>
@@ -977,12 +977,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$J$2:$J$6</f>
+              <f>'combined Stats-this session'!$J$2:$J$4</f>
             </numRef>
           </val>
         </ser>
@@ -1001,12 +1001,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$K$2:$K$6</f>
+              <f>'combined Stats-this session'!$K$2:$K$4</f>
             </numRef>
           </val>
         </ser>
@@ -1084,12 +1084,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$R$2:$R$6</f>
+              <f>'combined Stats-this session'!$R$2:$R$4</f>
             </numRef>
           </val>
         </ser>
@@ -1167,12 +1167,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$O$2:$O$6</f>
+              <f>'combined Stats-this session'!$O$2:$O$4</f>
             </numRef>
           </val>
         </ser>
@@ -1191,12 +1191,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$P$2:$P$6</f>
+              <f>'combined Stats-this session'!$P$2:$P$4</f>
             </numRef>
           </val>
         </ser>
@@ -1278,12 +1278,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'combined Stats-this session'!$A$2:$A$6</f>
+              <f>'combined Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'combined Stats-this session'!$Q$2:$Q$6</f>
+              <f>'combined Stats-this session'!$Q$2:$Q$4</f>
             </numRef>
           </val>
         </ser>
@@ -1360,12 +1360,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$F$2:$F$6</f>
+              <f>'NL Stats-this session'!$F$2:$F$4</f>
             </numRef>
           </val>
         </ser>
@@ -1384,12 +1384,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$G$2:$G$6</f>
+              <f>'NL Stats-this session'!$G$2:$G$4</f>
             </numRef>
           </val>
         </ser>
@@ -1408,12 +1408,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$H$2:$H$6</f>
+              <f>'NL Stats-this session'!$H$2:$H$4</f>
             </numRef>
           </val>
         </ser>
@@ -1487,12 +1487,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'NL Stats-this session'!$A$2:$A$6</f>
+              <f>'NL Stats-this session'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'NL Stats-this session'!$L$2:$L$6</f>
+              <f>'NL Stats-this session'!$L$2:$L$4</f>
             </numRef>
           </val>
         </ser>
@@ -2151,7 +2151,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2254,59 +2254,59 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Scott</t>
+          <t>Fish</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C2" t="n">
+        <v>53.59</v>
+      </c>
+      <c r="D2" t="n">
+        <v>33.59</v>
+      </c>
+      <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>-60</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
       <c r="F2" s="1" t="n">
-        <v>0.593</v>
+        <v>0.679</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0.324</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0.009299999999999999</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>0.538</v>
+        <v>0.118</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.157</v>
+        <v>0.268</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>0.065</v>
+        <v>0.19</v>
       </c>
       <c r="L2" t="n">
-        <v>2.88</v>
+        <v>0.19</v>
       </c>
       <c r="M2" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>66.05</v>
+        <v>112.17</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>48.34</v>
+        <v>66.58</v>
       </c>
       <c r="Q2" t="n">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>0.412</v>
+        <v>0.711</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -2321,234 +2321,118 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="C3" t="n">
-        <v>113.04</v>
+        <v>24.39</v>
       </c>
       <c r="D3" t="n">
-        <v>93.04000000000001</v>
+        <v>-26.61</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.471</v>
+        <v>0.466</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>0.336</v>
+        <v>0.31</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.0057</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0.449</v>
+        <v>0.454</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>0.184</v>
+        <v>0.126</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>0.099</v>
+        <v>0.046</v>
       </c>
       <c r="L3" t="n">
-        <v>2.75</v>
+        <v>3.68</v>
       </c>
       <c r="M3" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N3" t="n">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>230.44</v>
+        <v>41.7</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>137.24</v>
+        <v>58.54</v>
       </c>
       <c r="Q3" t="n">
-        <v>223</v>
+        <v>174</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>0.537</v>
+        <v>0.364</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>06/24/21</t>
+          <t>07/05/21</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cedric</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>37.74</v>
+        <v>13.02</v>
       </c>
       <c r="D4" t="n">
-        <v>-32.26</v>
+        <v>-6.98</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0.482</v>
+        <v>0.527</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0.174</v>
+        <v>0.513</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>0.197</v>
+        <v>0.22</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.093</v>
+        <v>0.08</v>
       </c>
       <c r="L4" t="n">
-        <v>0.41</v>
+        <v>3.16</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>112.42</v>
+        <v>43.65</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>33</v>
+        <v>64.11</v>
       </c>
       <c r="Q4" t="n">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0.474</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Cheyenne</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>20</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-20</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>0.372</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>0.044</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>0.153</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>0.175</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>0.073</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="M5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="n">
-        <v>6</v>
-      </c>
-      <c r="O5" s="2" t="n">
-        <v>45.16</v>
-      </c>
-      <c r="P5" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>137</v>
-      </c>
-      <c r="R5" s="1" t="n">
-        <v>0.417</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Fish</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>40</v>
-      </c>
-      <c r="C6" t="n">
-        <v>59.22</v>
-      </c>
-      <c r="D6" t="n">
-        <v>19.22</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>0.594</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>0.157</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>0.282</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>0.171</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2" t="n">
-        <v>140.72</v>
-      </c>
-      <c r="P6" s="2" t="n">
-        <v>43.39</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>170</v>
-      </c>
-      <c r="R6" s="1" t="n">
-        <v>0.604</v>
+        <v>0.364</v>
       </c>
     </row>
   </sheetData>
@@ -2563,7 +2447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2666,59 +2550,59 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Scott</t>
+          <t>Fish</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C2" t="n">
+        <v>53.59</v>
+      </c>
+      <c r="D2" t="n">
+        <v>33.59</v>
+      </c>
+      <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>-60</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
       <c r="F2" s="1" t="n">
-        <v>0.593</v>
+        <v>0.679</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0.324</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0.009299999999999999</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>0.538</v>
+        <v>0.118</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.157</v>
+        <v>0.268</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>0.065</v>
+        <v>0.19</v>
       </c>
       <c r="L2" t="n">
-        <v>2.88</v>
+        <v>0.19</v>
       </c>
       <c r="M2" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>66.05</v>
+        <v>112.17</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>48.34</v>
+        <v>66.58</v>
       </c>
       <c r="Q2" t="n">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>0.412</v>
+        <v>0.711</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -2733,234 +2617,118 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="C3" t="n">
-        <v>113.04</v>
+        <v>24.39</v>
       </c>
       <c r="D3" t="n">
-        <v>93.04000000000001</v>
+        <v>-26.61</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.471</v>
+        <v>0.466</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>0.336</v>
+        <v>0.31</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.0057</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0.449</v>
+        <v>0.454</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>0.184</v>
+        <v>0.126</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>0.099</v>
+        <v>0.046</v>
       </c>
       <c r="L3" t="n">
-        <v>2.75</v>
+        <v>3.68</v>
       </c>
       <c r="M3" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N3" t="n">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>230.44</v>
+        <v>41.7</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>137.24</v>
+        <v>58.54</v>
       </c>
       <c r="Q3" t="n">
-        <v>223</v>
+        <v>174</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>0.537</v>
+        <v>0.364</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>06/24/21</t>
+          <t>07/05/21</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cedric</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>37.74</v>
+        <v>13.02</v>
       </c>
       <c r="D4" t="n">
-        <v>-32.26</v>
+        <v>-6.98</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0.482</v>
+        <v>0.527</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0.174</v>
+        <v>0.513</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>0.197</v>
+        <v>0.22</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.093</v>
+        <v>0.08</v>
       </c>
       <c r="L4" t="n">
-        <v>0.41</v>
+        <v>3.16</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>112.42</v>
+        <v>43.65</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>33</v>
+        <v>64.11</v>
       </c>
       <c r="Q4" t="n">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0.474</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Cheyenne</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>20</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-20</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>0.372</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>0.044</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>0.153</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>0.175</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>0.073</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="M5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="n">
-        <v>6</v>
-      </c>
-      <c r="O5" s="2" t="n">
-        <v>45.16</v>
-      </c>
-      <c r="P5" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>137</v>
-      </c>
-      <c r="R5" s="1" t="n">
-        <v>0.417</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Fish</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>40</v>
-      </c>
-      <c r="C6" t="n">
-        <v>59.22</v>
-      </c>
-      <c r="D6" t="n">
-        <v>19.22</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>0.594</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>0.157</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>0.282</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>0.171</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2" t="n">
-        <v>140.72</v>
-      </c>
-      <c r="P6" s="2" t="n">
-        <v>43.39</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>170</v>
-      </c>
-      <c r="R6" s="1" t="n">
-        <v>0.604</v>
+        <v>0.364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>